<commit_message>
added customer class and added isNull() method to the excel class
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27002"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27004"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA6C264B-D75A-49FF-A9A7-F70D360C45F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFE9F97C-A24C-47F5-AF1D-15C92621BE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Customers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="19">
   <si>
     <t>Room #</t>
   </si>
@@ -61,10 +61,34 @@
     <t>penthouse</t>
   </si>
   <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>guns</t>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone #</t>
+  </si>
+  <si>
+    <t>works</t>
+  </si>
+  <si>
+    <t>Nathan</t>
+  </si>
+  <si>
+    <t>Wahba</t>
+  </si>
+  <si>
+    <t>nwahba02</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Nwahba</t>
   </si>
 </sst>
 </file>
@@ -101,8 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,294 +442,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="0">
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
         <v>100</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E2" s="0">
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="0">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
         <v>101</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E3" s="0">
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="0">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
         <v>102</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E4" s="0">
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="0">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
         <v>103</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E5" s="0">
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="0">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
         <v>104</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E6" s="0">
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
         <v>160</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="0">
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
         <v>105</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E7" s="0">
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="0">
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
         <v>106</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E8" s="0">
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="0">
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
         <v>107</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E9" s="0">
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="0">
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
         <v>108</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E10" s="0">
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="0">
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
         <v>200</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E11" s="0">
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="0">
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
         <v>201</v>
       </c>
-      <c r="C12" t="s" s="0">
+      <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E12" s="0">
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="0">
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
         <v>202</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E13" s="0">
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="0">
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
         <v>203</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D14" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E14" s="0">
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="0">
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
         <v>204</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D15" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E15" s="0">
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="0">
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
         <v>205</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E16" s="0">
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="0">
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
         <v>206</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E17" s="0">
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1">
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="0">
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
         <v>207</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D18" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E18" s="0">
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1">
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="0">
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
         <v>208</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D19" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E19" s="0">
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
         <v>224</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="0">
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
         <v>300</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D20" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="E20" s="0">
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1">
         <v>1000</v>
       </c>
     </row>
@@ -715,12 +737,238 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA349E6-1702-4F06-B76E-A2D7A0FA8AF9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="0">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a method to the Reservation Page Controller Class that saves the customer information to variables when they confirm their order.
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="27">
   <si>
     <t>Room #</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>4zU1J</t>
+  </si>
+  <si>
+    <t>9iOO1</t>
+  </si>
+  <si>
+    <t>kB0c7</t>
   </si>
 </sst>
 </file>
@@ -1134,10 +1140,40 @@
       <c r="A21" s="0">
         <v>20</v>
       </c>
+      <c r="B21" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s" s="0">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="0">
         <v>21</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:1">

</xml_diff>

<commit_message>
added date and room selection buttons as well as saving the values to variables
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="15">
   <si>
     <t>Room #</t>
   </si>
@@ -1302,283 +1302,283 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="2:6">
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2" t="s">
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3" t="s">
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27">
+      <c r="A27" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28">
+      <c r="A28" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29">
+      <c r="A29" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30">
+      <c r="A30" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31">
+      <c r="A31" s="0">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32">
+      <c r="A32" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33">
+      <c r="A33" s="0">
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34">
+      <c r="A34" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35">
+      <c r="A35" s="0">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36">
+      <c r="A36" s="0">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37">
+      <c r="A37" s="0">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38">
+      <c r="A38" s="0">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39">
+      <c r="A39" s="0">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40">
+      <c r="A40" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41">
+      <c r="A41" s="0">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42">
+      <c r="A42" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43">
+      <c r="A43" s="0">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44">
+      <c r="A44" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45">
+      <c r="A45" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46">
+      <c r="A46" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47">
+      <c r="A47" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48">
+      <c r="A48" s="0">
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49">
+      <c r="A49" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50">
+      <c r="A50" s="0">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51">
+      <c r="A51" s="0">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
merged with my branch
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19080" windowHeight="7140" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="19080" windowHeight="6045" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
   <si>
     <t>Room #</t>
   </si>
@@ -57,10 +57,58 @@
     <t>Phone #</t>
   </si>
   <si>
+    <t>Payment First Name</t>
+  </si>
+  <si>
+    <t>Payment Last Name</t>
+  </si>
+  <si>
+    <t>Card Number</t>
+  </si>
+  <si>
+    <t>Exp Date</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Jsmith12@gmail.com</t>
+  </si>
+  <si>
+    <t>12323451231</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>23423421</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>324432</t>
+  </si>
+  <si>
+    <t>AnLBq</t>
   </si>
 </sst>
 </file>
@@ -73,7 +121,14 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,138 +599,139 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -998,289 +1054,289 @@
   <sheetPr/>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>100</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2">
         <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>101</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>102</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
         <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>103</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
         <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>104</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
         <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>105</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>106</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
         <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>107</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
         <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>108</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
         <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>200</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
         <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>201</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
         <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>202</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
         <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>203</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2">
         <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>204</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
         <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>205</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="C16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2">
         <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>206</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
         <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>207</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2">
         <v>224</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>208</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2">
         <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>300</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2">
         <v>1000</v>
       </c>
     </row>
@@ -1293,53 +1349,93 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:6">
-      <c r="B1" t="s" s="0">
+    <row r="1" spans="2:12">
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
+      <c r="B2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>24</v>
+      </c>
       <c r="F2" t="s" s="0">
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
       <c r="F3" t="s" s="0">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1">

</xml_diff>

<commit_message>
first and last dates excel sheet
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -1,38 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27004"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0462F978-70BC-4F52-A6D8-6B31738FFE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="21735" windowHeight="4800" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
     <sheet name="Customers" sheetId="2" r:id="rId2"/>
+    <sheet name="Availability" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
+  <oleSize ref="A1:L51"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
   <si>
     <t>Room #</t>
   </si>
@@ -73,7 +58,7 @@
     <t>Phone #</t>
   </si>
   <si>
-    <t>Payment First Name</t>
+    <t>ID</t>
   </si>
   <si>
     <t>Payment Last Name</t>
@@ -91,31 +76,397 @@
     <t>Zip Code</t>
   </si>
   <si>
-    <t>ID</t>
+    <t/>
+  </si>
+  <si>
+    <t>10-20-23</t>
+  </si>
+  <si>
+    <t>10-21-23</t>
+  </si>
+  <si>
+    <t>10-22-23</t>
+  </si>
+  <si>
+    <t>10-23-23</t>
+  </si>
+  <si>
+    <t>10-24-23</t>
+  </si>
+  <si>
+    <t>10-25-23</t>
+  </si>
+  <si>
+    <t>10-26-23</t>
+  </si>
+  <si>
+    <t>10-27-23</t>
+  </si>
+  <si>
+    <t>10-28-23</t>
+  </si>
+  <si>
+    <t>10-29-23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -123,25 +474,311 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -190,7 +827,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -223,26 +860,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -275,23 +895,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -433,24 +1036,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -734,20 +1332,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA349E6-1702-4F06-B76E-A2D7A0FA8AF9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="2:12">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -779,80 +1379,98 @@
         <v>18</v>
       </c>
       <c r="L1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:1">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:1">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:1">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:1">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:1">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:1">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:1">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:1">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:1">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:1">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:1">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:1">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:1">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1034,5 +1652,108 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="2" width="11.4285714285714"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>100</v>
+      </c>
+      <c r="C1">
+        <v>101</v>
+      </c>
+      <c r="D1">
+        <v>102</v>
+      </c>
+      <c r="E1">
+        <v>200</v>
+      </c>
+      <c r="F1">
+        <v>201</v>
+      </c>
+      <c r="G1">
+        <v>202</v>
+      </c>
+      <c r="H1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
only first and last dates work
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21735" windowHeight="4800" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="19320" windowHeight="7905" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="32">
   <si>
     <t>Room #</t>
   </si>
@@ -79,34 +79,40 @@
     <t/>
   </si>
   <si>
-    <t>10-20-23</t>
-  </si>
-  <si>
-    <t>10-21-23</t>
-  </si>
-  <si>
-    <t>10-22-23</t>
-  </si>
-  <si>
-    <t>10-23-23</t>
-  </si>
-  <si>
-    <t>10-24-23</t>
-  </si>
-  <si>
-    <t>10-25-23</t>
-  </si>
-  <si>
-    <t>10-26-23</t>
-  </si>
-  <si>
-    <t>10-27-23</t>
-  </si>
-  <si>
-    <t>10-28-23</t>
-  </si>
-  <si>
-    <t>10-29-23</t>
+    <t>2023-10-23</t>
+  </si>
+  <si>
+    <t>booked</t>
+  </si>
+  <si>
+    <t>boooked</t>
+  </si>
+  <si>
+    <t>2023-10-24</t>
+  </si>
+  <si>
+    <t>2023-10-25</t>
+  </si>
+  <si>
+    <t>2023-10-26</t>
+  </si>
+  <si>
+    <t>2023-10-27</t>
+  </si>
+  <si>
+    <t>2023-10-28</t>
+  </si>
+  <si>
+    <t>2023-10-29</t>
+  </si>
+  <si>
+    <t>2023-10-30</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-11-01</t>
   </si>
 </sst>
 </file>
@@ -1342,7 +1348,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1382,27 +1388,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:1">
       <c r="A2">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -1410,88 +1398,370 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1659,10 +1929,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1671,9 +1941,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1">
         <v>100</v>
       </c>
@@ -1696,54 +1964,96 @@
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:1">
@@ -1751,6 +2061,57 @@
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
changed customer sheet to have their room information
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="12860" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="30240" windowHeight="12860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
   <si>
     <t>Room #</t>
   </si>
@@ -84,6 +84,9 @@
     <t>End Date</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>2023-10-23</t>
   </si>
   <si>
@@ -124,48 +127,6 @@
   </si>
   <si>
     <t>2023-11-05</t>
-  </si>
-  <si>
-    <t>booked</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Snow</t>
-  </si>
-  <si>
-    <t>jsnow@gmail.com</t>
-  </si>
-  <si>
-    <t>23412323434</t>
-  </si>
-  <si>
-    <t>nathan</t>
-  </si>
-  <si>
-    <t>wahba</t>
-  </si>
-  <si>
-    <t>23345234</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>90064</t>
-  </si>
-  <si>
-    <t>7eZHA</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>$115</t>
   </si>
 </sst>
 </file>
@@ -173,9 +134,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -187,8 +148,129 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -203,133 +285,12 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -346,6 +307,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -358,19 +331,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -382,145 +475,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,15 +492,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -554,15 +506,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -582,6 +525,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -589,6 +565,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -607,175 +592,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1400,345 +1361,333 @@
   <sheetPr/>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="2:16">
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s" s="0">
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s" s="0">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s" s="0">
+      <c r="M1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" t="s" s="0">
+      <c r="N1" t="s">
         <v>3</v>
       </c>
-      <c r="O1" t="s" s="0">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" t="s" s="0">
+      <c r="P1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="C2" t="s" s="0">
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="D2" t="s" s="0">
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="E2" t="s" s="0">
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="F2" t="s" s="0">
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="G2" t="s" s="0">
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="H2" t="s" s="0">
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="I2" t="s" s="0">
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="J2" t="s" s="0">
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="K2" t="s" s="0">
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="L2" t="s" s="0">
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="M2" t="s" s="0">
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="N2" t="s" s="0">
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="0">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="0">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="0">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="0">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="0">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="0">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="0">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="0">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="0">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="0">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="0">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="0">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="0">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="0">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="0">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="0">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="0">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="0">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="0">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="0">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="0">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="0">
-        <v>49</v>
-      </c>
-    </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="0">
+      <c r="A51">
         <v>50</v>
       </c>
     </row>
@@ -1751,115 +1700,106 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="2" width="11.4296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="1"/>
-      <c r="B1" s="0">
+      <c r="B1">
         <v>100</v>
       </c>
-      <c r="C1" s="0">
+      <c r="C1">
         <v>101</v>
       </c>
-      <c r="D1" s="0">
+      <c r="D1">
         <v>102</v>
       </c>
-      <c r="E1" s="0">
+      <c r="E1">
         <v>200</v>
       </c>
-      <c r="F1" s="0">
+      <c r="F1">
         <v>201</v>
       </c>
-      <c r="G1" s="0">
+      <c r="G1">
         <v>202</v>
-      </c>
-      <c r="H1" s="0">
-        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:1">

</xml_diff>

<commit_message>
the date and room type will now be sent between scenes, a blank review page is made for testing, added singleton classes to make instanced scenes.
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="12860" activeTab="1"/>
+    <workbookView windowWidth="21000" windowHeight="17010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
   <si>
     <t>Room #</t>
   </si>
@@ -84,10 +84,10 @@
     <t>End Date</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>2023-10-23</t>
+  </si>
+  <si>
+    <t>booked</t>
   </si>
   <si>
     <t>2023-10-24</t>
@@ -132,12 +132,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -156,8 +156,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -170,8 +171,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -185,29 +226,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -216,40 +234,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -257,14 +246,6 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -276,17 +257,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,13 +301,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,169 +475,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -492,36 +492,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -552,28 +522,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,151 +572,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -746,54 +746,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1068,7 +1068,7 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -1362,10 +1362,10 @@
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="2:16">
       <c r="B1" t="s">
@@ -1429,41 +1429,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:1">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6">
         <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:1">
@@ -1706,9 +1679,9 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="2" width="11.4296875"/>
+    <col min="1" max="2" width="11.4285714285714"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1732,8 +1705,14 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1752,14 +1731,26 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:1">

</xml_diff>

<commit_message>
working version of first sprint
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="12860" activeTab="1"/>
+    <workbookView windowWidth="19320" windowHeight="7395" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Availability" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:P51"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="44">
   <si>
     <t>Room #</t>
   </si>
@@ -57,7 +58,7 @@
     <t>Phone #</t>
   </si>
   <si>
-    <t>Payment First Name</t>
+    <t>ID</t>
   </si>
   <si>
     <t>Payment Last Name</t>
@@ -75,9 +76,6 @@
     <t>Zip Code</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Start Date</t>
   </si>
   <si>
@@ -87,12 +85,42 @@
     <t/>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>izEmP</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>$160</t>
+  </si>
+  <si>
     <t>2023-10-23</t>
   </si>
   <si>
+    <t>2023-11-01</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>UbiQJ</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
     <t>2023-10-24</t>
   </si>
   <si>
+    <t>2023-10-30</t>
+  </si>
+  <si>
     <t>2023-10-25</t>
   </si>
   <si>
@@ -108,13 +136,7 @@
     <t>2023-10-29</t>
   </si>
   <si>
-    <t>2023-10-30</t>
-  </si>
-  <si>
     <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
   </si>
   <si>
     <t>2023-11-02</t>
@@ -132,17 +154,45 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -156,8 +206,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -170,8 +221,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -185,29 +276,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -216,40 +284,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -257,14 +296,6 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -276,17 +307,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,13 +351,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,169 +525,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -492,36 +542,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -552,28 +572,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,208 +622,232 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1068,7 +1122,7 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -1361,11 +1415,16 @@
   <sheetPr/>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="10.5714285714286"/>
+    <col min="8" max="8" width="9.57142857142857"/>
+    <col min="16" max="16" width="11.4285714285714"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:16">
       <c r="B1" t="s">
@@ -1399,7 +1458,7 @@
         <v>18</v>
       </c>
       <c r="L1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
@@ -1408,20 +1467,107 @@
         <v>3</v>
       </c>
       <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1429,41 +1575,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:1">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6">
         <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:1">
@@ -1700,106 +1819,145 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="11.4296875"/>
+    <col min="1" max="2" width="11.4285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:20">
       <c r="A1" s="1"/>
-      <c r="B1">
+      <c r="B1" s="2">
         <v>100</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="2">
         <v>101</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="2">
         <v>102</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="2">
         <v>200</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="2">
         <v>201</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="2">
         <v>202</v>
+      </c>
+      <c r="H1" s="3">
+        <v>103</v>
+      </c>
+      <c r="I1" s="3">
+        <v>104</v>
+      </c>
+      <c r="J1" s="3">
+        <v>105</v>
+      </c>
+      <c r="K1" s="3">
+        <v>203</v>
+      </c>
+      <c r="L1" s="3">
+        <v>204</v>
+      </c>
+      <c r="M1" s="3">
+        <v>205</v>
+      </c>
+      <c r="N1" s="4">
+        <v>106</v>
+      </c>
+      <c r="O1" s="4">
+        <v>107</v>
+      </c>
+      <c r="P1" s="4">
+        <v>108</v>
+      </c>
+      <c r="Q1" s="4">
+        <v>206</v>
+      </c>
+      <c r="R1" s="4">
+        <v>207</v>
+      </c>
+      <c r="S1" s="4">
+        <v>208</v>
+      </c>
+      <c r="T1" s="5">
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:1">

</xml_diff>

<commit_message>
ground work for sprint 2 including new scenes
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
   <si>
     <t>Room #</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>End Date</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>2023-10-23</t>
@@ -1362,7 +1365,7 @@
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1414,9 +1417,28 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -1707,90 +1729,90 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:1">

</xml_diff>

<commit_message>
merged eric branch with nathan branch
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="12860" activeTab="2"/>
+    <workbookView windowWidth="30240" windowHeight="12860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -131,10 +131,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -182,15 +182,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,8 +226,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -214,67 +251,59 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,35 +316,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -326,13 +326,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,85 +488,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,79 +506,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,26 +520,56 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -564,51 +594,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -617,145 +602,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1390,8 +1390,8 @@
   <sheetPr/>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1709,8 +1709,8 @@
   <sheetPr/>
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:R20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
added missing changes from recent merge
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="12860" activeTab="1"/>
+    <workbookView windowWidth="21000" windowHeight="17010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>Room #</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>2023-10-29</t>
+  </si>
+  <si>
+    <t>booked</t>
   </si>
   <si>
     <t>2023-10-30</t>
@@ -129,12 +132,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -181,8 +184,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -196,119 +223,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -316,6 +230,95 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -326,25 +329,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -356,157 +503,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,11 +523,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,21 +572,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -570,35 +582,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,151 +600,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -775,54 +778,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1097,7 +1100,7 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -1391,14 +1394,14 @@
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="10.5703125"/>
-    <col min="8" max="8" width="9.5703125"/>
-    <col min="16" max="16" width="11.4296875"/>
+    <col min="6" max="6" width="10.5714285714286"/>
+    <col min="8" max="8" width="9.57142857142857"/>
+    <col min="16" max="16" width="11.4285714285714"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
@@ -1713,9 +1716,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="11.4296875"/>
+    <col min="1" max="2" width="11.4285714285714"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -1808,44 +1811,50 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="N8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:1">

</xml_diff>

<commit_message>
Fixed dates (always updates the excel file to current date)
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="17010" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9024" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
   <si>
     <t>Room #</t>
   </si>
@@ -83,61 +83,17 @@
   <si>
     <t>End Date</t>
   </si>
-  <si>
-    <t>2023-10-23</t>
-  </si>
-  <si>
-    <t>2023-10-24</t>
-  </si>
-  <si>
-    <t>2023-10-25</t>
-  </si>
-  <si>
-    <t>2023-10-26</t>
-  </si>
-  <si>
-    <t>2023-10-27</t>
-  </si>
-  <si>
-    <t>2023-10-28</t>
-  </si>
-  <si>
-    <t>2023-10-29</t>
-  </si>
-  <si>
-    <t>booked</t>
-  </si>
-  <si>
-    <t>2023-10-30</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
-    <t>2023-11-02</t>
-  </si>
-  <si>
-    <t>2023-11-03</t>
-  </si>
-  <si>
-    <t>2023-11-04</t>
-  </si>
-  <si>
-    <t>2023-11-05</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -768,13 +724,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1100,285 +1057,285 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1">
+      <c r="A2" s="6">
         <v>100</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="6">
         <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1">
+      <c r="A3" s="6">
         <v>101</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="6">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1">
+      <c r="A4" s="6">
         <v>102</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="6">
         <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1">
+      <c r="A5" s="6">
         <v>103</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="6">
         <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1">
+      <c r="A6" s="6">
         <v>104</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="6">
         <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1">
+      <c r="A7" s="6">
         <v>105</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="6">
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1">
+      <c r="A8" s="6">
         <v>106</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="6">
         <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1">
+      <c r="A9" s="6">
         <v>107</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="6">
         <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1">
+      <c r="A10" s="6">
         <v>108</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="6">
         <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1">
+      <c r="A11" s="6">
         <v>200</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="6">
         <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="1">
+      <c r="A12" s="6">
         <v>201</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="6">
         <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="1">
+      <c r="A13" s="6">
         <v>202</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="6">
         <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1">
+      <c r="A14" s="6">
         <v>203</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="6">
         <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="1">
+      <c r="A15" s="6">
         <v>204</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="6">
         <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="1">
+      <c r="A16" s="6">
         <v>205</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="6">
         <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="1">
+      <c r="A17" s="6">
         <v>206</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="6">
         <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="1">
+      <c r="A18" s="6">
         <v>207</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="6">
         <v>224</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="1">
+      <c r="A19" s="6">
         <v>208</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="6">
         <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="1">
+      <c r="A20" s="6">
         <v>300</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="6">
         <v>1000</v>
       </c>
     </row>
@@ -1393,15 +1350,16 @@
   <sheetPr/>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q2" sqref="B2:Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="10.5714285714286"/>
-    <col min="8" max="8" width="9.57142857142857"/>
-    <col min="16" max="16" width="11.4285714285714"/>
+    <col min="6" max="6" width="10.5740740740741"/>
+    <col min="8" max="8" width="9.57407407407407"/>
+    <col min="15" max="15" width="13.4444444444444" customWidth="1"/>
+    <col min="16" max="16" width="14.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
@@ -1710,19 +1668,19 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:T96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="11.4285714285714"/>
+    <col min="1" max="1" width="11.4259259259259" style="1"/>
+    <col min="2" max="2" width="11.4259259259259"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="1"/>
+    <row r="1" spans="2:20">
       <c r="B1" s="2">
         <v>100</v>
       </c>
@@ -1782,125 +1740,574 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
+      <c r="A2" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45231</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
+      <c r="A3" s="1">
+        <f ca="1">A2+1</f>
+        <v>45232</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
+      <c r="A4" s="1">
+        <f ca="1" t="shared" ref="A4:A15" si="0">A3+1</f>
+        <v>45233</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
+      <c r="A5" s="1">
+        <f ca="1" t="shared" si="0"/>
+        <v>45234</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
+      <c r="A6" s="1">
+        <f ca="1" t="shared" si="0"/>
+        <v>45235</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" t="s">
-        <v>29</v>
+      <c r="A7" s="1">
+        <f ca="1" t="shared" si="0"/>
+        <v>45236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1">
+        <f ca="1" t="shared" si="0"/>
+        <v>45237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1">
+        <f ca="1" t="shared" si="0"/>
+        <v>45238</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="1" t="s">
-        <v>31</v>
+      <c r="A10" s="1">
+        <f ca="1" t="shared" si="0"/>
+        <v>45239</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
+      <c r="A11" s="1">
+        <f ca="1" t="shared" si="0"/>
+        <v>45240</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
+      <c r="A12" s="1">
+        <f ca="1" t="shared" si="0"/>
+        <v>45241</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
+      <c r="A13" s="1">
+        <f ca="1" t="shared" si="0"/>
+        <v>45242</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="1" t="s">
-        <v>35</v>
+      <c r="A14" s="1">
+        <f ca="1" t="shared" si="0"/>
+        <v>45243</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="1" t="s">
-        <v>36</v>
+      <c r="A15" s="1">
+        <f ca="1" t="shared" si="0"/>
+        <v>45244</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <f ca="1" t="shared" ref="A16:A47" si="1">A15+1</f>
+        <v>45245</v>
+      </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45246</v>
+      </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45247</v>
+      </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45248</v>
+      </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45249</v>
+      </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45250</v>
+      </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45251</v>
+      </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45252</v>
+      </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45253</v>
+      </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45254</v>
+      </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45255</v>
+      </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45256</v>
+      </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45257</v>
+      </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45258</v>
+      </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45259</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45263</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45264</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45265</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45266</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45267</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45268</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45269</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45270</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45271</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45272</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45273</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45274</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45275</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="1">
+        <f ca="1" t="shared" si="1"/>
+        <v>45276</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="1">
+        <f ca="1" t="shared" ref="A48:A79" si="2">A47+1</f>
+        <v>45277</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45278</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45279</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45280</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45281</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45282</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45283</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45284</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45285</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45286</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45287</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45288</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45289</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45290</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45293</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45296</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45297</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45298</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45299</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45300</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45301</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45302</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45303</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45304</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45305</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45306</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45307</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="1">
+        <f ca="1" t="shared" si="2"/>
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="1">
+        <f ca="1" t="shared" ref="A80:A96" si="3">A79+1</f>
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45310</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45311</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45312</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45313</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45315</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45316</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45318</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45319</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45320</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45321</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45322</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45323</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45324</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="1">
+        <f ca="1" t="shared" si="3"/>
+        <v>45325</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed excel file so it always starts with todays date
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -1351,7 +1351,7 @@
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="B2:Q3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1671,7 +1671,7 @@
   <dimension ref="A1:T96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
working review page with users ID
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="12900" activeTab="2"/>
+    <workbookView windowWidth="19290" windowHeight="5085" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Availability" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:T135"/>
 </workbook>
 </file>
 
@@ -87,13 +88,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -132,33 +133,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -177,8 +164,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -193,46 +196,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,15 +213,44 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,7 +264,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,187 +286,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,17 +480,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -528,21 +529,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -557,13 +543,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -576,157 +566,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -736,54 +737,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1058,7 +1059,7 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
@@ -1352,16 +1353,16 @@
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:P9"/>
+      <selection activeCell="B2" sqref="B2:P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="10.5703125"/>
-    <col min="8" max="8" width="9.5703125"/>
+    <col min="6" max="6" width="10.5714285714286"/>
+    <col min="8" max="8" width="9.57142857142857"/>
     <col min="11" max="11" width="9" style="6"/>
-    <col min="15" max="15" width="13.4453125" customWidth="1"/>
-    <col min="16" max="16" width="14.3359375" customWidth="1"/>
+    <col min="15" max="15" width="13.447619047619" customWidth="1"/>
+    <col min="16" max="16" width="14.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
@@ -1450,20 +1451,6 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9" s="6"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
       <c r="P9" s="7"/>
     </row>
     <row r="10" spans="1:1">
@@ -1688,13 +1675,13 @@
   <dimension ref="A1:T135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B12"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.4296875" style="1"/>
-    <col min="2" max="2" width="11.4296875"/>
+    <col min="1" max="1" width="11.4285714285714" style="1"/>
+    <col min="2" max="2" width="11.4285714285714"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20">

</xml_diff>

<commit_message>
fixed erros and review page works
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19290" windowHeight="5085" activeTab="2"/>
+    <workbookView windowWidth="16110" windowHeight="7140" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -1353,7 +1353,7 @@
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1447,11 +1447,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:1">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="P9" s="7"/>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
@@ -1675,7 +1674,7 @@
   <dimension ref="A1:T135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
converted dates to String
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16110" windowHeight="7140" activeTab="2"/>
+    <workbookView windowWidth="30240" windowHeight="12900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Availability" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:T135"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
   <si>
     <t>Room #</t>
   </si>
@@ -83,18 +82,66 @@
   </si>
   <si>
     <t>End Date</t>
+  </si>
+  <si>
+    <t>booked</t>
+  </si>
+  <si>
+    <t>kdsjfkldsj</t>
+  </si>
+  <si>
+    <t>sjfdjslkfn</t>
+  </si>
+  <si>
+    <t>asms</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>fsdakjf</t>
+  </si>
+  <si>
+    <t>dkjfsdjf</t>
+  </si>
+  <si>
+    <t>12344</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>sdjkfn</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>CSzVL</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>$115</t>
+  </si>
+  <si>
+    <t>2023-11-14</t>
+  </si>
+  <si>
+    <t>2023-11-17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -141,9 +188,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -156,27 +202,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -196,21 +225,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -219,16 +233,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,8 +262,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,17 +308,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -286,37 +333,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -328,73 +483,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,67 +513,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,21 +524,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -528,6 +560,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -558,6 +601,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -566,168 +624,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -737,54 +784,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1059,7 +1106,7 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
@@ -1352,313 +1399,358 @@
   <sheetPr/>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:P9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="B2:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="6" max="6" width="10.5714285714286"/>
-    <col min="8" max="8" width="9.57142857142857"/>
-    <col min="11" max="11" width="9" style="6"/>
-    <col min="15" max="15" width="13.447619047619" customWidth="1"/>
-    <col min="16" max="16" width="14.3333333333333" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125"/>
+    <col min="8" max="8" width="9.5703125"/>
+    <col min="11" max="11" style="6" width="9.0"/>
+    <col min="15" max="15" customWidth="true" width="13.4453125"/>
+    <col min="16" max="16" customWidth="true" width="14.3359375"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
+      <c r="B2" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s" s="6">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s" s="0">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27">
+      <c r="A27" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28">
+      <c r="A28" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29">
+      <c r="A29" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30">
+      <c r="A30" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31">
+      <c r="A31" s="0">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32">
+      <c r="A32" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33">
+      <c r="A33" s="0">
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34">
+      <c r="A34" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35">
+      <c r="A35" s="0">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36">
+      <c r="A36" s="0">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37">
+      <c r="A37" s="0">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38">
+      <c r="A38" s="0">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39">
+      <c r="A39" s="0">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40">
+      <c r="A40" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41">
+      <c r="A41" s="0">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42">
+      <c r="A42" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43">
+      <c r="A43" s="0">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44">
+      <c r="A44" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45">
+      <c r="A45" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46">
+      <c r="A46" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47">
+      <c r="A47" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48">
+      <c r="A48" s="0">
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49">
+      <c r="A49" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50">
+      <c r="A50" s="0">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51">
+      <c r="A51" s="0">
         <v>50</v>
       </c>
     </row>
@@ -1673,14 +1765,14 @@
   <sheetPr/>
   <dimension ref="A1:T135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="11.4285714285714" style="1"/>
-    <col min="2" max="2" width="11.4285714285714"/>
+    <col min="1" max="1" style="1" width="11.4296875"/>
+    <col min="2" max="2" width="11.4296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20">
@@ -1811,20 +1903,32 @@
       <c r="A15" s="1">
         <v>45244</v>
       </c>
+      <c r="B15" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1">
         <v>45245</v>
       </c>
+      <c r="B16" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1">
         <v>45246</v>
       </c>
+      <c r="B17" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1">
         <v>45247</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:1">

</xml_diff>

<commit_message>
changed all the ints to string
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="89">
   <si>
     <t>Room #</t>
   </si>
@@ -130,6 +130,159 @@
   </si>
   <si>
     <t>2023-11-17</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>snow</t>
+  </si>
+  <si>
+    <t>jnso</t>
+  </si>
+  <si>
+    <t>sdajfnds</t>
+  </si>
+  <si>
+    <t>sdkjfndsfj</t>
+  </si>
+  <si>
+    <t>Y07ZX</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>2023-11-18</t>
+  </si>
+  <si>
+    <t>VNVNVN</t>
+  </si>
+  <si>
+    <t>dvnksl</t>
+  </si>
+  <si>
+    <t>djsknfjksdn</t>
+  </si>
+  <si>
+    <t>1234432</t>
+  </si>
+  <si>
+    <t>asdfkjsd</t>
+  </si>
+  <si>
+    <t>sadfkj</t>
+  </si>
+  <si>
+    <t>adsfk</t>
+  </si>
+  <si>
+    <t>askdjf</t>
+  </si>
+  <si>
+    <t>zu7or</t>
+  </si>
+  <si>
+    <t>2023-11-21</t>
+  </si>
+  <si>
+    <t>2023-11-24</t>
+  </si>
+  <si>
+    <t>adsjfn</t>
+  </si>
+  <si>
+    <t>jvndskj</t>
+  </si>
+  <si>
+    <t>nwahba</t>
+  </si>
+  <si>
+    <t>adsjfj</t>
+  </si>
+  <si>
+    <t>djkfndsj</t>
+  </si>
+  <si>
+    <t>1212</t>
+  </si>
+  <si>
+    <t>sdkjfn</t>
+  </si>
+  <si>
+    <t>1235</t>
+  </si>
+  <si>
+    <t>WLlfm</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>2023-11-07</t>
+  </si>
+  <si>
+    <t>adsfkln</t>
+  </si>
+  <si>
+    <t>sdfklnfds</t>
+  </si>
+  <si>
+    <t>sndjkfn</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>dskfjn</t>
+  </si>
+  <si>
+    <t>12/12</t>
+  </si>
+  <si>
+    <t>dskjfns</t>
+  </si>
+  <si>
+    <t>1233</t>
+  </si>
+  <si>
+    <t>t2hoS</t>
+  </si>
+  <si>
+    <t>2023-11-28</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
+  </si>
+  <si>
+    <t>adskf</t>
+  </si>
+  <si>
+    <t>SDKLFNSDK</t>
+  </si>
+  <si>
+    <t>dsjfn</t>
+  </si>
+  <si>
+    <t>dsfjds</t>
+  </si>
+  <si>
+    <t>dskjfsn</t>
+  </si>
+  <si>
+    <t>dskjfnsd</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>WXdJ4</t>
+  </si>
+  <si>
+    <t>102</t>
   </si>
 </sst>
 </file>
@@ -1513,25 +1666,242 @@
       <c r="A3" s="0">
         <v>2</v>
       </c>
+      <c r="B3" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="6"/>
+      <c r="L3" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="O3" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="P3" t="s" s="0">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="0">
         <v>3</v>
       </c>
+      <c r="B4" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="K4" t="s" s="6">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="N4" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="O4" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="P4" t="s" s="0">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="0">
         <v>4</v>
       </c>
+      <c r="B5" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="K5" t="s" s="6">
+        <v>64</v>
+      </c>
+      <c r="L5" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="M5" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="N5" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="O5" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="P5" t="s" s="0">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="0">
         <v>5</v>
       </c>
+      <c r="B6" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="K6" t="s" s="6">
+        <v>76</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="O6" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="0">
         <v>6</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="K7" t="s" s="6">
+        <v>86</v>
+      </c>
+      <c r="L7" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="M7" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="N7" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="O7" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="P7" t="s" s="0">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1868,36 +2238,57 @@
       <c r="A8" s="1">
         <v>45237</v>
       </c>
+      <c r="N8" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1">
         <v>45238</v>
       </c>
+      <c r="N9" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1">
         <v>45239</v>
       </c>
+      <c r="N10" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1">
         <v>45240</v>
       </c>
+      <c r="N11" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1">
         <v>45241</v>
       </c>
+      <c r="N12" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1">
         <v>45242</v>
       </c>
+      <c r="N13" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1">
         <v>45243</v>
       </c>
+      <c r="N14" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1">
@@ -1906,6 +2297,15 @@
       <c r="B15" t="s" s="0">
         <v>22</v>
       </c>
+      <c r="C15" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="N15" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1">
@@ -1914,6 +2314,15 @@
       <c r="B16" t="s" s="0">
         <v>22</v>
       </c>
+      <c r="C16" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="N16" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1">
@@ -1922,6 +2331,15 @@
       <c r="B17" t="s" s="0">
         <v>22</v>
       </c>
+      <c r="C17" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="N17" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1">
@@ -1930,11 +2348,26 @@
       <c r="B18" t="s" s="0">
         <v>22</v>
       </c>
+      <c r="C18" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="N18" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1">
         <v>45248</v>
       </c>
+      <c r="C19" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="N19" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1">
@@ -1950,21 +2383,33 @@
       <c r="A22" s="1">
         <v>45251</v>
       </c>
+      <c r="B22" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1">
         <v>45252</v>
       </c>
+      <c r="B23" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1">
         <v>45253</v>
       </c>
+      <c r="B24" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1">
         <v>45254</v>
       </c>
+      <c r="B25" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1">
@@ -1985,15 +2430,24 @@
       <c r="A29" s="1">
         <v>45258</v>
       </c>
+      <c r="B29" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1">
         <v>45259</v>
       </c>
+      <c r="B30" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="1">
         <v>45260</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:1">

</xml_diff>

<commit_message>
check available on search page works
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="12900" activeTab="1"/>
+    <workbookView windowWidth="30240" windowHeight="12900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="89">
   <si>
     <t>Room #</t>
   </si>
@@ -84,205 +84,205 @@
     <t>End Date</t>
   </si>
   <si>
+    <t>kdsjfkldsj</t>
+  </si>
+  <si>
+    <t>sjfdjslkfn</t>
+  </si>
+  <si>
+    <t>asms</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>fsdakjf</t>
+  </si>
+  <si>
+    <t>dkjfsdjf</t>
+  </si>
+  <si>
+    <t>12344</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>sdjkfn</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>CSzVL</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>$115</t>
+  </si>
+  <si>
+    <t>2023-11-14</t>
+  </si>
+  <si>
+    <t>2023-11-17</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>snow</t>
+  </si>
+  <si>
+    <t>jnso</t>
+  </si>
+  <si>
+    <t>sdajfnds</t>
+  </si>
+  <si>
+    <t>sdkjfndsfj</t>
+  </si>
+  <si>
+    <t>Y07ZX</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>2023-11-18</t>
+  </si>
+  <si>
+    <t>VNVNVN</t>
+  </si>
+  <si>
+    <t>dvnksl</t>
+  </si>
+  <si>
+    <t>djsknfjksdn</t>
+  </si>
+  <si>
+    <t>1234432</t>
+  </si>
+  <si>
+    <t>asdfkjsd</t>
+  </si>
+  <si>
+    <t>sadfkj</t>
+  </si>
+  <si>
+    <t>adsfk</t>
+  </si>
+  <si>
+    <t>askdjf</t>
+  </si>
+  <si>
+    <t>zu7or</t>
+  </si>
+  <si>
+    <t>2023-11-21</t>
+  </si>
+  <si>
+    <t>2023-11-24</t>
+  </si>
+  <si>
+    <t>adsjfn</t>
+  </si>
+  <si>
+    <t>jvndskj</t>
+  </si>
+  <si>
+    <t>nwahba</t>
+  </si>
+  <si>
+    <t>adsjfj</t>
+  </si>
+  <si>
+    <t>djkfndsj</t>
+  </si>
+  <si>
+    <t>1212</t>
+  </si>
+  <si>
+    <t>sdkjfn</t>
+  </si>
+  <si>
+    <t>1235</t>
+  </si>
+  <si>
+    <t>WLlfm</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>2023-11-07</t>
+  </si>
+  <si>
+    <t>adsfkln</t>
+  </si>
+  <si>
+    <t>sdfklnfds</t>
+  </si>
+  <si>
+    <t>sndjkfn</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>dskfjn</t>
+  </si>
+  <si>
+    <t>12/12</t>
+  </si>
+  <si>
+    <t>dskjfns</t>
+  </si>
+  <si>
+    <t>1233</t>
+  </si>
+  <si>
+    <t>t2hoS</t>
+  </si>
+  <si>
+    <t>2023-11-28</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
+  </si>
+  <si>
+    <t>adskf</t>
+  </si>
+  <si>
+    <t>SDKLFNSDK</t>
+  </si>
+  <si>
+    <t>dsjfn</t>
+  </si>
+  <si>
+    <t>dsfjds</t>
+  </si>
+  <si>
+    <t>dskjfsn</t>
+  </si>
+  <si>
+    <t>dskjfnsd</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>WXdJ4</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
     <t>booked</t>
-  </si>
-  <si>
-    <t>kdsjfkldsj</t>
-  </si>
-  <si>
-    <t>sjfdjslkfn</t>
-  </si>
-  <si>
-    <t>asms</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>fsdakjf</t>
-  </si>
-  <si>
-    <t>dkjfsdjf</t>
-  </si>
-  <si>
-    <t>12344</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>sdjkfn</t>
-  </si>
-  <si>
-    <t>12345</t>
-  </si>
-  <si>
-    <t>CSzVL</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>$115</t>
-  </si>
-  <si>
-    <t>2023-11-14</t>
-  </si>
-  <si>
-    <t>2023-11-17</t>
-  </si>
-  <si>
-    <t>john</t>
-  </si>
-  <si>
-    <t>snow</t>
-  </si>
-  <si>
-    <t>jnso</t>
-  </si>
-  <si>
-    <t>sdajfnds</t>
-  </si>
-  <si>
-    <t>sdkjfndsfj</t>
-  </si>
-  <si>
-    <t>Y07ZX</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>2023-11-18</t>
-  </si>
-  <si>
-    <t>VNVNVN</t>
-  </si>
-  <si>
-    <t>dvnksl</t>
-  </si>
-  <si>
-    <t>djsknfjksdn</t>
-  </si>
-  <si>
-    <t>1234432</t>
-  </si>
-  <si>
-    <t>asdfkjsd</t>
-  </si>
-  <si>
-    <t>sadfkj</t>
-  </si>
-  <si>
-    <t>adsfk</t>
-  </si>
-  <si>
-    <t>askdjf</t>
-  </si>
-  <si>
-    <t>zu7or</t>
-  </si>
-  <si>
-    <t>2023-11-21</t>
-  </si>
-  <si>
-    <t>2023-11-24</t>
-  </si>
-  <si>
-    <t>adsjfn</t>
-  </si>
-  <si>
-    <t>jvndskj</t>
-  </si>
-  <si>
-    <t>nwahba</t>
-  </si>
-  <si>
-    <t>adsjfj</t>
-  </si>
-  <si>
-    <t>djkfndsj</t>
-  </si>
-  <si>
-    <t>1212</t>
-  </si>
-  <si>
-    <t>sdkjfn</t>
-  </si>
-  <si>
-    <t>1235</t>
-  </si>
-  <si>
-    <t>WLlfm</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>224</t>
-  </si>
-  <si>
-    <t>2023-11-07</t>
-  </si>
-  <si>
-    <t>adsfkln</t>
-  </si>
-  <si>
-    <t>sdfklnfds</t>
-  </si>
-  <si>
-    <t>sndjkfn</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>dskfjn</t>
-  </si>
-  <si>
-    <t>12/12</t>
-  </si>
-  <si>
-    <t>dskjfns</t>
-  </si>
-  <si>
-    <t>1233</t>
-  </si>
-  <si>
-    <t>t2hoS</t>
-  </si>
-  <si>
-    <t>2023-11-28</t>
-  </si>
-  <si>
-    <t>2023-11-30</t>
-  </si>
-  <si>
-    <t>adskf</t>
-  </si>
-  <si>
-    <t>SDKLFNSDK</t>
-  </si>
-  <si>
-    <t>dsjfn</t>
-  </si>
-  <si>
-    <t>dsfjds</t>
-  </si>
-  <si>
-    <t>dskjfsn</t>
-  </si>
-  <si>
-    <t>dskjfnsd</t>
-  </si>
-  <si>
-    <t>234</t>
-  </si>
-  <si>
-    <t>WXdJ4</t>
-  </si>
-  <si>
-    <t>102</t>
   </si>
 </sst>
 </file>
@@ -290,11 +290,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -341,8 +341,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -355,6 +402,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -370,15 +441,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -392,90 +476,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -483,6 +483,102 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -492,7 +588,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -504,19 +624,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -528,37 +648,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -570,103 +666,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -680,11 +680,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -713,17 +719,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -739,17 +734,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -772,6 +763,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -780,142 +780,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -927,7 +927,7 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1552,7 +1552,7 @@
   <sheetPr/>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P2" sqref="B2:P2"/>
     </sheetView>
   </sheetViews>
@@ -1560,567 +1560,563 @@
   <cols>
     <col min="6" max="6" width="10.5703125"/>
     <col min="8" max="8" width="9.5703125"/>
-    <col min="11" max="11" style="6" width="9.0"/>
-    <col min="15" max="15" customWidth="true" width="13.4453125"/>
-    <col min="16" max="16" customWidth="true" width="14.3359375"/>
+    <col min="11" max="11" width="9" style="6"/>
+    <col min="15" max="15" width="13.4453125" customWidth="1"/>
+    <col min="16" max="16" width="14.3359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s" s="0">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s" s="0">
+      <c r="M1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" t="s" s="0">
+      <c r="N1" t="s">
         <v>3</v>
       </c>
-      <c r="O1" t="s" s="0">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" t="s" s="0">
+      <c r="P1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="0">
+    <row r="2" spans="1:16">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="F2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="G2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="H2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="I2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="J2" t="s">
         <v>30</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="K2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s" s="6">
+      <c r="L2" t="s">
         <v>32</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="M2" t="s">
         <v>33</v>
       </c>
-      <c r="M2" t="s" s="0">
+      <c r="N2" t="s">
         <v>34</v>
       </c>
-      <c r="N2" t="s" s="0">
+      <c r="O2" t="s">
         <v>35</v>
       </c>
-      <c r="O2" t="s" s="0">
+      <c r="P2" t="s">
         <v>36</v>
       </c>
-      <c r="P2" t="s" s="0">
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="0">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L5" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N5" t="s">
+        <v>66</v>
+      </c>
+      <c r="O5" t="s">
+        <v>67</v>
+      </c>
+      <c r="P5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="F3" t="s" s="0">
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="G3" t="s" s="0">
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0"/>
-      <c r="K3" s="6"/>
-      <c r="L3" t="s" s="0">
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="M3" t="s" s="0">
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="N3" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="O3" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="P3" t="s" s="0">
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="0">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s" s="0">
+    <row r="47" spans="1:1">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="C4" t="s" s="0">
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="D4" t="s" s="0">
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="E4" t="s" s="0">
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50">
         <v>49</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="K4" t="s" s="6">
-        <v>32</v>
-      </c>
-      <c r="L4" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="M4" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="N4" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="O4" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="P4" t="s" s="0">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="0">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>59</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>62</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>63</v>
-      </c>
-      <c r="K5" t="s" s="6">
-        <v>64</v>
-      </c>
-      <c r="L5" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="M5" t="s" s="0">
-        <v>66</v>
-      </c>
-      <c r="N5" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="O5" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="P5" t="s" s="0">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="0">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>73</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>74</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>75</v>
-      </c>
-      <c r="K6" t="s" s="6">
-        <v>76</v>
-      </c>
-      <c r="L6" t="s" s="0">
-        <v>77</v>
-      </c>
-      <c r="M6" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="N6" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="O6" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="P6" t="s" s="0">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="0">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>80</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>81</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>83</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>74</v>
-      </c>
-      <c r="J7" t="s" s="0">
-        <v>85</v>
-      </c>
-      <c r="K7" t="s" s="6">
-        <v>86</v>
-      </c>
-      <c r="L7" t="s" s="0">
-        <v>87</v>
-      </c>
-      <c r="M7" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="N7" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="O7" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="P7" t="s" s="0">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="0">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="0">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="0">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="0">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="0">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="0">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="0">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="0">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="0">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="0">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="0">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="0">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="0">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="0">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="0">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="0">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="0">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="0">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="0">
-        <v>49</v>
-      </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="0">
+      <c r="A51">
         <v>50</v>
       </c>
     </row>
@@ -2135,13 +2131,13 @@
   <sheetPr/>
   <dimension ref="A1:T135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B2:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" style="1" width="11.4296875"/>
+    <col min="1" max="1" width="11.4296875" style="1"/>
     <col min="2" max="2" width="11.4296875"/>
   </cols>
   <sheetData>
@@ -2234,144 +2230,243 @@
         <v>45236</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>45237</v>
       </c>
-      <c r="N8" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="N8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="N9" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="N9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>45239</v>
       </c>
-      <c r="N10" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="N10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>45240</v>
       </c>
-      <c r="N11" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="N11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>45241</v>
       </c>
-      <c r="N12" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="N12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>45242</v>
       </c>
-      <c r="N13" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="N13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>45243</v>
       </c>
-      <c r="N14" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="N14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="1">
         <v>45244</v>
       </c>
-      <c r="B15" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="N15" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" t="s">
+        <v>88</v>
+      </c>
+      <c r="N15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1">
         <v>45245</v>
       </c>
-      <c r="B16" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="N16" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" t="s">
+        <v>88</v>
+      </c>
+      <c r="J16" t="s">
+        <v>88</v>
+      </c>
+      <c r="N16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="1">
         <v>45246</v>
       </c>
-      <c r="B17" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="D17" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="N17" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" t="s">
+        <v>88</v>
+      </c>
+      <c r="I17" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" t="s">
+        <v>88</v>
+      </c>
+      <c r="N17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="1">
         <v>45247</v>
       </c>
-      <c r="B18" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="N18" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" t="s">
+        <v>88</v>
+      </c>
+      <c r="J18" t="s">
+        <v>88</v>
+      </c>
+      <c r="N18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="1">
         <v>45248</v>
       </c>
-      <c r="C19" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="N19" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="C19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" t="s">
+        <v>88</v>
+      </c>
+      <c r="J19" t="s">
+        <v>88</v>
+      </c>
+      <c r="N19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>45249</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:1">
@@ -2379,36 +2474,36 @@
         <v>45250</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:2">
       <c r="A22" s="1">
         <v>45251</v>
       </c>
-      <c r="B22" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="1">
         <v>45252</v>
       </c>
-      <c r="B23" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="1">
         <v>45253</v>
       </c>
-      <c r="B24" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="1">
         <v>45254</v>
       </c>
-      <c r="B25" t="s" s="0">
-        <v>22</v>
+      <c r="B25" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:1">
@@ -2426,28 +2521,28 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:2">
       <c r="A29" s="1">
         <v>45258</v>
       </c>
-      <c r="B29" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="1">
         <v>45259</v>
       </c>
-      <c r="B30" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="1">
         <v>45260</v>
       </c>
-      <c r="B31" t="s" s="0">
-        <v>22</v>
+      <c r="B31" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:1">

</xml_diff>

<commit_message>
added teh change reservation gui and controller
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="101">
   <si>
     <t>Room #</t>
   </si>
@@ -283,6 +283,42 @@
   </si>
   <si>
     <t>booked</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h/i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>KM2VC</t>
+  </si>
+  <si>
+    <t>2023-11-09</t>
   </si>
 </sst>
 </file>
@@ -290,11 +326,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -1560,563 +1596,608 @@
   <cols>
     <col min="6" max="6" width="10.5703125"/>
     <col min="8" max="8" width="9.5703125"/>
-    <col min="11" max="11" width="9" style="6"/>
-    <col min="15" max="15" width="13.4453125" customWidth="1"/>
-    <col min="16" max="16" width="14.3359375" customWidth="1"/>
+    <col min="11" max="11" style="6" width="9.0"/>
+    <col min="15" max="15" customWidth="true" width="13.4453125"/>
+    <col min="16" max="16" customWidth="true" width="14.3359375"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>30</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" t="s" s="0">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>52</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" t="s" s="0">
         <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>62</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>74</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>76</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" t="s" s="0">
         <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>84</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" t="s" s="0">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
+      <c r="B8" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="K8" t="s" s="6">
+        <v>98</v>
+      </c>
+      <c r="L8" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="M8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N8" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="P8" t="s" s="0">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27">
+      <c r="A27" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28">
+      <c r="A28" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29">
+      <c r="A29" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30">
+      <c r="A30" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31">
+      <c r="A31" s="0">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32">
+      <c r="A32" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33">
+      <c r="A33" s="0">
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34">
+      <c r="A34" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35">
+      <c r="A35" s="0">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36">
+      <c r="A36" s="0">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37">
+      <c r="A37" s="0">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38">
+      <c r="A38" s="0">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39">
+      <c r="A39" s="0">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40">
+      <c r="A40" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41">
+      <c r="A41" s="0">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42">
+      <c r="A42" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43">
+      <c r="A43" s="0">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44">
+      <c r="A44" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45">
+      <c r="A45" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46">
+      <c r="A46" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47">
+      <c r="A47" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48">
+      <c r="A48" s="0">
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49">
+      <c r="A49" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50">
+      <c r="A50" s="0">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51">
+      <c r="A51" s="0">
         <v>50</v>
       </c>
     </row>
@@ -2137,7 +2218,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="11.4296875" style="1"/>
+    <col min="1" max="1" style="1" width="11.4296875"/>
     <col min="2" max="2" width="11.4296875"/>
   </cols>
   <sheetData>
@@ -2234,7 +2315,10 @@
       <c r="A8" s="1">
         <v>45237</v>
       </c>
-      <c r="N8" t="s">
+      <c r="B8" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="N8" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2242,7 +2326,10 @@
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="N9" t="s">
+      <c r="B9" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="N9" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2250,7 +2337,10 @@
       <c r="A10" s="1">
         <v>45239</v>
       </c>
-      <c r="N10" t="s">
+      <c r="B10" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="N10" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2258,7 +2348,7 @@
       <c r="A11" s="1">
         <v>45240</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2266,7 +2356,7 @@
       <c r="A12" s="1">
         <v>45241</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2274,7 +2364,7 @@
       <c r="A13" s="1">
         <v>45242</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2282,7 +2372,7 @@
       <c r="A14" s="1">
         <v>45243</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2290,34 +2380,34 @@
       <c r="A15" s="1">
         <v>45244</v>
       </c>
-      <c r="B15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" t="s">
-        <v>88</v>
-      </c>
-      <c r="H15" t="s">
-        <v>88</v>
-      </c>
-      <c r="I15" t="s">
-        <v>88</v>
-      </c>
-      <c r="J15" t="s">
-        <v>88</v>
-      </c>
-      <c r="N15" t="s">
+      <c r="B15" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="H15" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="I15" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="J15" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="N15" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2325,34 +2415,34 @@
       <c r="A16" s="1">
         <v>45245</v>
       </c>
-      <c r="B16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" t="s">
-        <v>88</v>
-      </c>
-      <c r="F16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" t="s">
-        <v>88</v>
-      </c>
-      <c r="H16" t="s">
-        <v>88</v>
-      </c>
-      <c r="I16" t="s">
-        <v>88</v>
-      </c>
-      <c r="J16" t="s">
-        <v>88</v>
-      </c>
-      <c r="N16" t="s">
+      <c r="B16" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="G16" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="H16" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="I16" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="J16" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="N16" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2360,34 +2450,34 @@
       <c r="A17" s="1">
         <v>45246</v>
       </c>
-      <c r="B17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" t="s">
-        <v>88</v>
-      </c>
-      <c r="H17" t="s">
-        <v>88</v>
-      </c>
-      <c r="I17" t="s">
-        <v>88</v>
-      </c>
-      <c r="J17" t="s">
-        <v>88</v>
-      </c>
-      <c r="N17" t="s">
+      <c r="B17" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="G17" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="H17" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="I17" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="J17" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="N17" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2395,34 +2485,34 @@
       <c r="A18" s="1">
         <v>45247</v>
       </c>
-      <c r="B18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" t="s">
-        <v>88</v>
-      </c>
-      <c r="H18" t="s">
-        <v>88</v>
-      </c>
-      <c r="I18" t="s">
-        <v>88</v>
-      </c>
-      <c r="J18" t="s">
-        <v>88</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="B18" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="G18" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="H18" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="I18" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="J18" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="N18" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2430,28 +2520,28 @@
       <c r="A19" s="1">
         <v>45248</v>
       </c>
-      <c r="C19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" t="s">
-        <v>88</v>
-      </c>
-      <c r="G19" t="s">
-        <v>88</v>
-      </c>
-      <c r="H19" t="s">
-        <v>88</v>
-      </c>
-      <c r="I19" t="s">
-        <v>88</v>
-      </c>
-      <c r="J19" t="s">
-        <v>88</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="C19" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="F19" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="G19" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="H19" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="I19" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="J19" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="N19" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2459,13 +2549,13 @@
       <c r="A20" s="1">
         <v>45249</v>
       </c>
-      <c r="E20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="E20" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="F20" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="G20" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2478,7 +2568,7 @@
       <c r="A22" s="1">
         <v>45251</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2486,7 +2576,7 @@
       <c r="A23" s="1">
         <v>45252</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2494,7 +2584,7 @@
       <c r="A24" s="1">
         <v>45253</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2502,7 +2592,7 @@
       <c r="A25" s="1">
         <v>45254</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2525,7 +2615,7 @@
       <c r="A29" s="1">
         <v>45258</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2533,7 +2623,7 @@
       <c r="A30" s="1">
         <v>45259</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -2541,7 +2631,7 @@
       <c r="A31" s="1">
         <v>45260</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="s" s="0">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change,cancel methods added and added more documentation
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,80 +4,58 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="12900" activeTab="2"/>
+    <workbookView windowWidth="30240" windowHeight="12900"/>
   </bookViews>
   <sheets>
-    <sheet name="Rooms" sheetId="1" r:id="rId1"/>
-    <sheet name="Customers" sheetId="2" r:id="rId2"/>
-    <sheet name="Availability" sheetId="3" r:id="rId3"/>
+    <sheet name="Customers" sheetId="2" r:id="rId1"/>
+    <sheet name="Availability" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="100">
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone #</t>
+  </si>
+  <si>
+    <t>Payment First Name</t>
+  </si>
+  <si>
+    <t>Payment Last Name</t>
+  </si>
+  <si>
+    <t>Card Number</t>
+  </si>
+  <si>
+    <t>Exp Date</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>Room #</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Availibilty</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
-    <t>single</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>double</t>
-  </si>
-  <si>
-    <t>king</t>
-  </si>
-  <si>
-    <t>penthouse</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone #</t>
-  </si>
-  <si>
-    <t>Payment First Name</t>
-  </si>
-  <si>
-    <t>Payment Last Name</t>
-  </si>
-  <si>
-    <t>Card Number</t>
-  </si>
-  <si>
-    <t>Exp Date</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Zip Code</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Start Date</t>
   </si>
   <si>
@@ -282,43 +260,61 @@
     <t>102</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h/i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>KM2VC</t>
+  </si>
+  <si>
+    <t>2023-11-09</t>
+  </si>
+  <si>
     <t>booked</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h/i</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>KM2VC</t>
-  </si>
-  <si>
-    <t>2023-11-09</t>
+    <t>sdjf</t>
+  </si>
+  <si>
+    <t>dsjfhs</t>
+  </si>
+  <si>
+    <t>dssjfsdj</t>
+  </si>
+  <si>
+    <t>djfhds</t>
+  </si>
+  <si>
+    <t>dsjfhds</t>
+  </si>
+  <si>
+    <t>UJqhv</t>
   </si>
 </sst>
 </file>
@@ -328,9 +324,9 @@
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -386,33 +382,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -423,18 +396,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -453,9 +419,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -469,6 +456,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -477,18 +479,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -499,17 +501,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -528,13 +524,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,163 +698,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,7 +731,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -755,6 +751,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -766,17 +782,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -800,158 +805,149 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -961,15 +957,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1289,306 +1284,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="7">
-        <v>100</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="7">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7">
-        <v>101</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="7">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="7">
-        <v>102</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="7">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="7">
-        <v>103</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="7">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="7">
-        <v>104</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="7">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="7">
-        <v>105</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="7">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="7">
-        <v>106</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="7">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="7">
-        <v>107</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="7">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="7">
-        <v>108</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="7">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="7">
-        <v>200</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="7">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="7">
-        <v>201</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="7">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="7">
-        <v>202</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="7">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="7">
-        <v>203</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="7">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="7">
-        <v>204</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="7">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="7">
-        <v>205</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="7">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="7">
-        <v>206</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="7">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="7">
-        <v>207</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="7">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="7">
-        <v>208</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="7">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="7">
-        <v>300</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="7">
-        <v>1000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P2" sqref="B2:P2"/>
     </sheetView>
   </sheetViews>
@@ -1603,49 +1301,49 @@
   <sheetData>
     <row r="1" spans="2:16">
       <c r="B1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="L1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="M1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="N1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="O1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="P1" t="s" s="0">
         <v>14</v>
-      </c>
-      <c r="H1" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="N1" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="O1" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="P1" t="s" s="0">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1653,49 +1351,49 @@
         <v>1</v>
       </c>
       <c r="B2" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="J2" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="K2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="L2" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="M2" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="N2" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="O2" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="P2" t="s" s="0">
         <v>29</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="M2" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="N2" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="O2" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="P2" t="s" s="0">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1703,37 +1401,37 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s" s="0">
         <v>37</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="L3" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="M3" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="N3" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="O3" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="P3" t="s" s="0">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1741,49 +1439,49 @@
         <v>3</v>
       </c>
       <c r="B4" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="K4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="M4" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="N4" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="P4" t="s" s="0">
         <v>48</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="M4" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="N4" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="O4" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="P4" t="s" s="0">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1791,49 +1489,49 @@
         <v>4</v>
       </c>
       <c r="B5" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="L5" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="M5" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="E5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s" s="0">
+      <c r="N5" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="G5" t="s" s="0">
+      <c r="O5" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="H5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>62</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="L5" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="M5" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="N5" t="s" s="0">
-        <v>66</v>
-      </c>
-      <c r="O5" t="s" s="0">
-        <v>67</v>
-      </c>
       <c r="P5" t="s" s="0">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1841,49 +1539,49 @@
         <v>5</v>
       </c>
       <c r="B6" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="L6" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="M6" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="O6" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="E6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s" s="0">
+      <c r="P6" t="s" s="0">
         <v>71</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>73</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>74</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="L6" t="s" s="0">
-        <v>76</v>
-      </c>
-      <c r="M6" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="N6" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="O6" t="s" s="0">
-        <v>77</v>
-      </c>
-      <c r="P6" t="s" s="0">
-        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1891,104 +1589,149 @@
         <v>6</v>
       </c>
       <c r="B7" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="M7" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="D7" t="s" s="0">
-        <v>81</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>83</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>63</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>73</v>
-      </c>
-      <c r="J7" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="L7" t="s" s="0">
-        <v>86</v>
-      </c>
-      <c r="M7" t="s" s="0">
-        <v>87</v>
-      </c>
       <c r="N7" t="s" s="0">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="O7" t="s" s="0">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="P7" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="0">
         <v>7</v>
       </c>
       <c r="B8" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="J8" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="K8" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="L8" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="M8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="N8" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="P8" t="s" s="0">
         <v>92</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>93</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>94</v>
-      </c>
-      <c r="H8" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="I8" t="s" s="0">
-        <v>96</v>
-      </c>
-      <c r="J8" t="s" s="0">
-        <v>97</v>
-      </c>
-      <c r="K8" t="s" s="6">
-        <v>98</v>
-      </c>
-      <c r="L8" t="s" s="0">
-        <v>99</v>
-      </c>
-      <c r="M8" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="N8" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="O8" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="P8" t="s" s="0">
-        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="0">
         <v>8</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="K9" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="M9" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="N9" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="O9" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="P9" t="s" s="0">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -2207,12 +1950,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:T135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -2316,10 +2059,10 @@
         <v>45237</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="N8" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -2327,10 +2070,10 @@
         <v>45238</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="N9" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -2338,10 +2081,10 @@
         <v>45239</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="N10" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -2349,7 +2092,7 @@
         <v>45240</v>
       </c>
       <c r="N11" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -2357,7 +2100,7 @@
         <v>45241</v>
       </c>
       <c r="N12" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -2365,7 +2108,7 @@
         <v>45242</v>
       </c>
       <c r="N13" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -2373,7 +2116,7 @@
         <v>45243</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -2381,34 +2124,34 @@
         <v>45244</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F15" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G15" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H15" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="I15" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="J15" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="N15" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -2416,34 +2159,34 @@
         <v>45245</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F16" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H16" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="I16" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="J16" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="N16" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -2451,34 +2194,34 @@
         <v>45246</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G17" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H17" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="I17" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="J17" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="N17" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -2486,34 +2229,34 @@
         <v>45247</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F18" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G18" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H18" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="I18" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="J18" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="N18" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -2521,28 +2264,28 @@
         <v>45248</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F19" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H19" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="J19" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="N19" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2550,13 +2293,13 @@
         <v>45249</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F20" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G20" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:1">
@@ -2569,7 +2312,10 @@
         <v>45251</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2577,7 +2323,10 @@
         <v>45252</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2585,7 +2334,10 @@
         <v>45253</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2593,7 +2345,10 @@
         <v>45254</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:1">
@@ -2616,7 +2371,7 @@
         <v>45258</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2624,7 +2379,7 @@
         <v>45259</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -2632,7 +2387,7 @@
         <v>45260</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:1">

</xml_diff>

<commit_message>
changed the send email to its own method
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>First Name</t>
   </si>
@@ -108,6 +108,75 @@
   </si>
   <si>
     <t>2023-11-09</t>
+  </si>
+  <si>
+    <t>dsjfds</t>
+  </si>
+  <si>
+    <t>dsfkjds</t>
+  </si>
+  <si>
+    <t>kjsdfns</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>asdfkn</t>
+  </si>
+  <si>
+    <t>dskfjn</t>
+  </si>
+  <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t>sndfm</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>9N1i6</t>
+  </si>
+  <si>
+    <t>2023-11-15</t>
+  </si>
+  <si>
+    <t>2023-11-18</t>
+  </si>
+  <si>
+    <t>adsfkjhds</t>
+  </si>
+  <si>
+    <t>sdfjkdsfh</t>
+  </si>
+  <si>
+    <t>nwahba02@gmail.com</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>dsjfh</t>
+  </si>
+  <si>
+    <t>sdkjfh</t>
+  </si>
+  <si>
+    <t>2345</t>
+  </si>
+  <si>
+    <t>fndsjkf</t>
+  </si>
+  <si>
+    <t>R2RZa</t>
+  </si>
+  <si>
+    <t>2023-11-22</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
   </si>
 </sst>
 </file>
@@ -1193,10 +1262,100 @@
       <c r="A3" s="0">
         <v>2</v>
       </c>
+      <c r="B3" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s" s="6">
+        <v>39</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="P3" t="s" s="0">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="0">
         <v>3</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="K4" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="N4" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="P4" t="s" s="0">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -1594,21 +1753,33 @@
       <c r="A16" s="1">
         <v>45245</v>
       </c>
+      <c r="B16" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1">
         <v>45246</v>
       </c>
+      <c r="B17" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1">
         <v>45247</v>
       </c>
+      <c r="B18" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1">
         <v>45248</v>
       </c>
+      <c r="B19" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1">
@@ -1629,45 +1800,72 @@
       <c r="A23" s="1">
         <v>45252</v>
       </c>
+      <c r="B23" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1">
         <v>45253</v>
       </c>
+      <c r="B24" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1">
         <v>45254</v>
       </c>
+      <c r="B25" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1">
         <v>45255</v>
       </c>
+      <c r="B26" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1">
         <v>45256</v>
       </c>
+      <c r="B27" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1">
         <v>45257</v>
       </c>
+      <c r="B28" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1">
         <v>45258</v>
       </c>
+      <c r="B29" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1">
         <v>45259</v>
       </c>
+      <c r="B30" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="1">
         <v>45260</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:1">

</xml_diff>

<commit_message>
edit page shows SOME information
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="142">
   <si>
     <t>First Name</t>
   </si>
@@ -294,6 +294,153 @@
   </si>
   <si>
     <t>KjLkx</t>
+  </si>
+  <si>
+    <t>ushfdj</t>
+  </si>
+  <si>
+    <t>djsfh</t>
+  </si>
+  <si>
+    <t>qjksh</t>
+  </si>
+  <si>
+    <t>asdfn</t>
+  </si>
+  <si>
+    <t>dsjkfb</t>
+  </si>
+  <si>
+    <t>12/21</t>
+  </si>
+  <si>
+    <t>sdkf</t>
+  </si>
+  <si>
+    <t>IuDAH</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>2023-11-20</t>
+  </si>
+  <si>
+    <t>2023-11-24</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>ssdfkj</t>
+  </si>
+  <si>
+    <t>sdafn</t>
+  </si>
+  <si>
+    <t>sdkjfn</t>
+  </si>
+  <si>
+    <t>dsfmn</t>
+  </si>
+  <si>
+    <t>zz4i1</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>2023-11-25</t>
+  </si>
+  <si>
+    <t>ajsdnfjk</t>
+  </si>
+  <si>
+    <t>dsjkhfjsdhf</t>
+  </si>
+  <si>
+    <t>njwsenaj</t>
+  </si>
+  <si>
+    <t>asdfhjsabf</t>
+  </si>
+  <si>
+    <t>dsjbf</t>
+  </si>
+  <si>
+    <t>12344</t>
+  </si>
+  <si>
+    <t>kjsdfhb</t>
+  </si>
+  <si>
+    <t>JPfkp</t>
+  </si>
+  <si>
+    <t>2023-12-06</t>
+  </si>
+  <si>
+    <t>2023-12-07</t>
+  </si>
+  <si>
+    <t>nathan</t>
+  </si>
+  <si>
+    <t>wahba</t>
+  </si>
+  <si>
+    <t>skdjf</t>
+  </si>
+  <si>
+    <t>asdkjf</t>
+  </si>
+  <si>
+    <t>12/23</t>
+  </si>
+  <si>
+    <t>sdfkjn</t>
+  </si>
+  <si>
+    <t>GCIWf</t>
+  </si>
+  <si>
+    <t>2023-11-21</t>
+  </si>
+  <si>
+    <t>askdfj</t>
+  </si>
+  <si>
+    <t>sdlkfj</t>
+  </si>
+  <si>
+    <t>qwaj</t>
+  </si>
+  <si>
+    <t>asdfkjn</t>
+  </si>
+  <si>
+    <t>sdjkfn</t>
+  </si>
+  <si>
+    <t>kdsj</t>
+  </si>
+  <si>
+    <t>jDLqF</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>$160</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-29</t>
   </si>
 </sst>
 </file>
@@ -1679,25 +1826,250 @@
       <c r="A9" s="0">
         <v>8</v>
       </c>
+      <c r="B9" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="K9" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="L9" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="M9" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="N9" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="O9" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="P9" t="s" s="0">
+        <v>103</v>
+      </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="0">
         <v>9</v>
       </c>
+      <c r="B10" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="K10" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="L10" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="M10" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="N10" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="O10" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="P10" t="s" s="0">
+        <v>112</v>
+      </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="0">
         <v>10</v>
       </c>
+      <c r="B11" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>116</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>118</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="J11" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="K11" t="s" s="6">
+        <v>34</v>
+      </c>
+      <c r="L11" t="s" s="0">
+        <v>120</v>
+      </c>
+      <c r="M11" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="N11" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="O11" t="s" s="0">
+        <v>121</v>
+      </c>
+      <c r="P11" t="s" s="0">
+        <v>122</v>
+      </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="0">
         <v>11</v>
       </c>
+      <c r="B12" t="s" s="0">
+        <v>123</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>124</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>127</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="K12" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="L12" t="s" s="0">
+        <v>129</v>
+      </c>
+      <c r="M12" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="N12" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="O12" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="P12" t="s" s="0">
+        <v>130</v>
+      </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="0">
         <v>12</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>131</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>132</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>135</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="K13" t="s" s="6">
+        <v>34</v>
+      </c>
+      <c r="L13" t="s" s="0">
+        <v>137</v>
+      </c>
+      <c r="M13" t="s" s="0">
+        <v>138</v>
+      </c>
+      <c r="N13" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="O13" t="s" s="0">
+        <v>140</v>
+      </c>
+      <c r="P13" t="s" s="0">
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -2099,11 +2471,29 @@
       <c r="A21" s="1">
         <v>45250</v>
       </c>
+      <c r="B21" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1">
         <v>45251</v>
       </c>
+      <c r="B22" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1">
@@ -2112,6 +2502,12 @@
       <c r="B23" t="s" s="0">
         <v>15</v>
       </c>
+      <c r="C23" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1">
@@ -2120,6 +2516,12 @@
       <c r="B24" t="s" s="0">
         <v>15</v>
       </c>
+      <c r="C24" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1">
@@ -2128,6 +2530,12 @@
       <c r="B25" t="s" s="0">
         <v>15</v>
       </c>
+      <c r="C25" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1">
@@ -2136,6 +2544,9 @@
       <c r="B26" t="s" s="0">
         <v>15</v>
       </c>
+      <c r="D26" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1">
@@ -2152,6 +2563,9 @@
       <c r="B28" t="s" s="0">
         <v>15</v>
       </c>
+      <c r="H28" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1">
@@ -2160,6 +2574,9 @@
       <c r="B29" t="s" s="0">
         <v>15</v>
       </c>
+      <c r="H29" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1">
@@ -2168,6 +2585,9 @@
       <c r="B30" t="s" s="0">
         <v>15</v>
       </c>
+      <c r="H30" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="1">
@@ -2206,10 +2626,16 @@
       <c r="A37" s="1">
         <v>45266</v>
       </c>
+      <c r="B37" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1">
         <v>45267</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:1">

</xml_diff>

<commit_message>
First batch of changes today include adding labels to all errors, adding ui elements to edit page, pop up will now close on action, 5 digit reservation number.
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>First Name</t>
   </si>
@@ -94,6 +94,42 @@
   </si>
   <si>
     <t>booked</t>
+  </si>
+  <si>
+    <t>eric</t>
+  </si>
+  <si>
+    <t>rubio</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>12311111111</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>10/25</t>
+  </si>
+  <si>
+    <t>usa</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>dbRaT</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
   </si>
 </sst>
 </file>
@@ -1149,6 +1185,51 @@
       <c r="A3" s="0">
         <v>2</v>
       </c>
+      <c r="B3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s" s="6">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="O3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s" s="0">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="0">
@@ -1487,6 +1568,9 @@
       <c r="B4" t="s" s="0">
         <v>25</v>
       </c>
+      <c r="N4" t="s" s="0">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
@@ -1495,6 +1579,9 @@
       <c r="B5" t="s" s="0">
         <v>25</v>
       </c>
+      <c r="N5" t="s" s="0">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
@@ -1503,6 +1590,9 @@
       <c r="B6" t="s" s="0">
         <v>25</v>
       </c>
+      <c r="N6" t="s" s="0">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
@@ -1511,20 +1601,32 @@
       <c r="B7" t="s" s="0">
         <v>25</v>
       </c>
+      <c r="N7" t="s" s="0">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1">
         <v>45251</v>
       </c>
+      <c r="N8" t="s" s="0">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1">
         <v>45252</v>
       </c>
+      <c r="N9" t="s" s="0">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1">
         <v>45253</v>
+      </c>
+      <c r="N10" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:1">

</xml_diff>

<commit_message>
second batch of changes today. fixed the multiple pop up instances in a round about way
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>First Name</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>10/24</t>
   </si>
 </sst>
 </file>
@@ -1207,7 +1210,7 @@
         <v>30</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s" s="0">
         <v>32</v>
@@ -1218,18 +1221,10 @@
       <c r="L3" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="M3" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="N3" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="O3" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="P3" t="s" s="0">
-        <v>37</v>
-      </c>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
+      <c r="P3" s="0"/>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="0">

</xml_diff>

<commit_message>
changed the pop up sequence to the best of my abilities
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16110" windowHeight="5805"/>
+    <workbookView windowHeight="17610"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="2" r:id="rId1"/>
     <sheet name="Availability" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:T136"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="45">
   <si>
     <t>First Name</t>
   </si>
@@ -63,76 +62,94 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>adsf</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>12334</t>
-  </si>
-  <si>
-    <t>12/23</t>
-  </si>
-  <si>
-    <t>asdfasdf</t>
-  </si>
-  <si>
-    <t>bbbbb</t>
-  </si>
-  <si>
-    <t>100</t>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>Rubio</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>1/1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>xwwae</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>2023-11-17</t>
+  </si>
+  <si>
+    <t>2023-11-25</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>booked</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8/9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>DbSOr</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>5/6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>zSiee</t>
+  </si>
+  <si>
+    <t>102</t>
   </si>
   <si>
     <t>$115</t>
   </si>
   <si>
-    <t>2023-11-17</t>
-  </si>
-  <si>
-    <t>2023-11-20</t>
-  </si>
-  <si>
-    <t>booked</t>
-  </si>
-  <si>
-    <t>eric</t>
-  </si>
-  <si>
-    <t>rubio</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>12311111111</t>
-  </si>
-  <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>10/25</t>
-  </si>
-  <si>
-    <t>usa</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>dbRaT</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>224</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>10/24</t>
+    <t>2023-11-18</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1122,7 @@
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1168,82 +1185,261 @@
       <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-      <c r="I2" s="0"/>
-      <c r="J2" s="0"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="0"/>
-      <c r="M2" s="0"/>
-      <c r="N2" s="0"/>
-      <c r="O2" s="0"/>
-      <c r="P2" s="0"/>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="0">
         <v>2</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>38</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I3" s="0"/>
       <c r="J3" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="K3" t="s" s="6">
-        <v>33</v>
-      </c>
-      <c r="L3" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="M3" s="0"/>
-      <c r="N3" s="0"/>
-      <c r="O3" s="0"/>
-      <c r="P3" s="0"/>
-    </row>
-    <row r="4" spans="1:1">
+        <v>25</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="0"/>
+      <c r="M3" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="0">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="I4" s="0"/>
+      <c r="J4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="0"/>
+      <c r="M4" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="0">
         <v>4</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="I5" s="0"/>
+      <c r="J5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="0"/>
+      <c r="M5" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="0">
         <v>5</v>
       </c>
+      <c r="B6" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="K6" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="O6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="0">
         <v>6</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="K7" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="L7" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="M7" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="N7" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="O7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="P7" t="s" s="0">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1556,82 +1752,160 @@
         <v>45246</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>45247</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>26</v>
       </c>
       <c r="N4" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>26</v>
+      </c>
+      <c r="O4" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P4" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>45248</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>26</v>
       </c>
       <c r="N5" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>26</v>
+      </c>
+      <c r="O5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P5" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1">
         <v>45249</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>26</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>26</v>
+      </c>
+      <c r="O6" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1">
         <v>45250</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>26</v>
       </c>
       <c r="N7" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+        <v>26</v>
+      </c>
+      <c r="O7" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P7" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1">
         <v>45251</v>
       </c>
+      <c r="C8" t="s" s="0">
+        <v>26</v>
+      </c>
       <c r="N8" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>26</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P8" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1">
         <v>45252</v>
       </c>
+      <c r="C9" t="s" s="0">
+        <v>26</v>
+      </c>
       <c r="N9" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+        <v>26</v>
+      </c>
+      <c r="O9" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P9" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1">
         <v>45253</v>
       </c>
+      <c r="C10" t="s" s="0">
+        <v>26</v>
+      </c>
       <c r="N10" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+        <v>26</v>
+      </c>
+      <c r="O10" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P10" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1">
         <v>45254</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="C11" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="O11" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
         <v>45255</v>
+      </c>
+      <c r="O12" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:1">

</xml_diff>

<commit_message>
added the extra info on excel
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17610"/>
+    <workbookView windowWidth="17370" windowHeight="6360"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="2" r:id="rId1"/>
     <sheet name="Availability" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:P51"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
   <si>
     <t>First Name</t>
   </si>
@@ -47,12 +48,18 @@
     <t>Zip Code</t>
   </si>
   <si>
+    <t>Sec Code</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
     <t>Room #</t>
   </si>
   <si>
+    <t>Room Size</t>
+  </si>
+  <si>
     <t>Price</t>
   </si>
   <si>
@@ -62,94 +69,130 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>Eric</t>
-  </si>
-  <si>
-    <t>Rubio</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>1/1</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>xwwae</t>
-  </si>
-  <si>
-    <t>107</t>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>asdfas</t>
+  </si>
+  <si>
+    <t>3423</t>
+  </si>
+  <si>
+    <t>23/12</t>
+  </si>
+  <si>
+    <t>sdafsad</t>
+  </si>
+  <si>
+    <t>1234344</t>
+  </si>
+  <si>
+    <t>332</t>
+  </si>
+  <si>
+    <t>4UKbo</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>$115</t>
+  </si>
+  <si>
+    <t>2023-11-21</t>
+  </si>
+  <si>
+    <t>2023-11-25</t>
+  </si>
+  <si>
+    <t>sadf</t>
+  </si>
+  <si>
+    <t>asdfdsaf</t>
+  </si>
+  <si>
+    <t>1233</t>
+  </si>
+  <si>
+    <t>asdfdsa</t>
+  </si>
+  <si>
+    <t>asdfdsf</t>
+  </si>
+  <si>
+    <t>12/23</t>
+  </si>
+  <si>
+    <t>432</t>
+  </si>
+  <si>
+    <t>mG259</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>2023-11-20</t>
+  </si>
+  <si>
+    <t>2023-11-24</t>
+  </si>
+  <si>
+    <t>dssdd</t>
+  </si>
+  <si>
+    <t>asdfsadf</t>
+  </si>
+  <si>
+    <t>12312</t>
+  </si>
+  <si>
+    <t>23/23</t>
+  </si>
+  <si>
+    <t>dsafdasf</t>
+  </si>
+  <si>
+    <t>UNA01</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>booked</t>
+  </si>
+  <si>
+    <t>adfa</t>
+  </si>
+  <si>
+    <t>asdfadsf</t>
+  </si>
+  <si>
+    <t>123213</t>
+  </si>
+  <si>
+    <t>adsfadsf</t>
+  </si>
+  <si>
+    <t>ej6iw</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>King</t>
   </si>
   <si>
     <t>224</t>
   </si>
   <si>
-    <t>2023-11-17</t>
-  </si>
-  <si>
-    <t>2023-11-25</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>booked</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8/9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>DbSOr</t>
-  </si>
-  <si>
-    <t>108</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>5/6</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>zSiee</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>$115</t>
-  </si>
-  <si>
-    <t>2023-11-18</t>
+    <t>2023-11-28</t>
   </si>
 </sst>
 </file>
@@ -1119,10 +1162,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1134,7 +1177,7 @@
     <col min="16" max="16" customWidth="true" width="14.3333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16">
+    <row r="1" spans="2:18">
       <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
@@ -1180,266 +1223,245 @@
       <c r="P1" t="s" s="0">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="0">
         <v>1</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="O2" t="s" s="0">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="P2" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>28</v>
+      </c>
+      <c r="Q2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="R2" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="0">
         <v>2</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="I3" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>36</v>
+      </c>
       <c r="J3" t="s" s="0">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>37</v>
+      </c>
       <c r="M3" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>38</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="O3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="P3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="Q3" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="R3" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="0">
         <v>3</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="I4" s="0"/>
+        <v>44</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>45</v>
+      </c>
       <c r="J4" t="s" s="0">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>37</v>
+      </c>
       <c r="M4" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>47</v>
+      </c>
+      <c r="N4" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="O4" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="P4" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="Q4" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="R4" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" s="0">
         <v>4</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="I5" s="0"/>
+        <v>52</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>45</v>
+      </c>
       <c r="J5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="0"/>
+        <v>53</v>
+      </c>
+      <c r="K5" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s" s="0">
+        <v>18</v>
+      </c>
       <c r="M5" t="s" s="0">
-        <v>25</v>
+        <v>54</v>
+      </c>
+      <c r="N5" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="O5" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="P5" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="Q5" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="R5" t="s" s="0">
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="K6" t="s" s="6">
-        <v>35</v>
-      </c>
-      <c r="L6" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="M6" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="N6" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="O6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="P6" t="s" s="0">
-        <v>38</v>
-      </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="0">
         <v>6</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="J7" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="K7" t="s" s="6">
-        <v>40</v>
-      </c>
-      <c r="L7" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="M7" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="N7" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="O7" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="P7" t="s" s="0">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1674,7 +1696,7 @@
   <dimension ref="A1:T136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1752,175 +1774,88 @@
         <v>45246</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:1">
       <c r="A4" s="1">
         <v>45247</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="N4" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="O4" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P4" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" s="1">
         <v>45248</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="N5" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="O5" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P5" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" s="1">
         <v>45249</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="N6" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="O6" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P6" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:1">
       <c r="A7" s="1">
         <v>45250</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="N7" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="O7" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P7" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+    </row>
+    <row r="8" spans="1:1">
       <c r="A8" s="1">
         <v>45251</v>
       </c>
-      <c r="C8" t="s" s="0">
-        <v>26</v>
-      </c>
       <c r="N8" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="O8" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P8" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
       <c r="A9" s="1">
         <v>45252</v>
       </c>
-      <c r="C9" t="s" s="0">
-        <v>26</v>
-      </c>
       <c r="N9" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="O9" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P9" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
       <c r="A10" s="1">
         <v>45253</v>
       </c>
-      <c r="C10" t="s" s="0">
-        <v>26</v>
-      </c>
       <c r="N10" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="O10" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P10" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
       <c r="A11" s="1">
         <v>45254</v>
       </c>
-      <c r="C11" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="O11" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="N11" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
       <c r="A12" s="1">
         <v>45255</v>
       </c>
-      <c r="O12" t="s" s="0">
-        <v>26</v>
+      <c r="N12" t="s" s="0">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1">
         <v>45256</v>
       </c>
+      <c r="N13" t="s" s="0">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1">
         <v>45257</v>
       </c>
+      <c r="N14" t="s" s="0">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1">
         <v>45258</v>
+      </c>
+      <c r="N15" t="s" s="0">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:1">

</xml_diff>

<commit_message>
edit button and dates work
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="81">
   <si>
     <t>First Name</t>
   </si>
@@ -193,6 +193,72 @@
   </si>
   <si>
     <t>2023-11-28</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>asdffd</t>
+  </si>
+  <si>
+    <t>0H1Tb</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>$160</t>
+  </si>
+  <si>
+    <t>adsf</t>
+  </si>
+  <si>
+    <t>12/32</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>05J79</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>asdfsdaf</t>
+  </si>
+  <si>
+    <t>dsfa1</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>sadfsda</t>
+  </si>
+  <si>
+    <t>sdafas</t>
+  </si>
+  <si>
+    <t>12321</t>
+  </si>
+  <si>
+    <t>23/43</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>uBydR</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
   </si>
 </sst>
 </file>
@@ -1458,15 +1524,166 @@
       <c r="A6" s="0">
         <v>5</v>
       </c>
+      <c r="B6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="K6" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="O6" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="Q6" s="0"/>
+      <c r="R6" t="s" s="0">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="0">
         <v>6</v>
       </c>
+      <c r="B7" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="M7" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="N7" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="O7" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="P7" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="Q7" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="R7" t="s" s="0">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="0">
         <v>7</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="M8" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="N8" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="P8" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="Q8" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="R8" t="s" s="0">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -1793,6 +2010,9 @@
       <c r="A7" s="1">
         <v>45250</v>
       </c>
+      <c r="O7" t="s" s="0">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1">
@@ -1801,6 +2021,9 @@
       <c r="N8" t="s" s="0">
         <v>49</v>
       </c>
+      <c r="O8" t="s" s="0">
+        <v>49</v>
+      </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1">
@@ -1809,6 +2032,9 @@
       <c r="N9" t="s" s="0">
         <v>49</v>
       </c>
+      <c r="O9" t="s" s="0">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1">
@@ -1817,6 +2043,9 @@
       <c r="N10" t="s" s="0">
         <v>49</v>
       </c>
+      <c r="O10" t="s" s="0">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1">
@@ -1825,6 +2054,9 @@
       <c r="N11" t="s" s="0">
         <v>49</v>
       </c>
+      <c r="O11" t="s" s="0">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1">
@@ -1854,6 +2086,9 @@
       <c r="A15" s="1">
         <v>45258</v>
       </c>
+      <c r="H15" t="s" s="0">
+        <v>49</v>
+      </c>
       <c r="N15" t="s" s="0">
         <v>49</v>
       </c>
@@ -1862,10 +2097,16 @@
       <c r="A16" s="1">
         <v>45259</v>
       </c>
+      <c r="H16" t="s" s="0">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1">
         <v>45260</v>
+      </c>
+      <c r="H17" t="s" s="0">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:1">

</xml_diff>

<commit_message>
Email changes on reserve class and total cost on reservation page controller class
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17370" windowHeight="6360"/>
+    <workbookView windowWidth="23040" windowHeight="8580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="2" r:id="rId1"/>
     <sheet name="Availability" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:P51"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="90">
   <si>
     <t>First Name</t>
   </si>
@@ -165,100 +164,127 @@
     <t>200</t>
   </si>
   <si>
+    <t>adfa</t>
+  </si>
+  <si>
+    <t>asdfadsf</t>
+  </si>
+  <si>
+    <t>123213</t>
+  </si>
+  <si>
+    <t>adsfadsf</t>
+  </si>
+  <si>
+    <t>ej6iw</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>2023-11-28</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>asdffd</t>
+  </si>
+  <si>
+    <t>0H1Tb</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>$160</t>
+  </si>
+  <si>
+    <t>adsf</t>
+  </si>
+  <si>
+    <t>12/32</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>05J79</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>asdfsdaf</t>
+  </si>
+  <si>
+    <t>dsfa1</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>sadfsda</t>
+  </si>
+  <si>
+    <t>sdafas</t>
+  </si>
+  <si>
+    <t>12321</t>
+  </si>
+  <si>
+    <t>23/43</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>uBydR</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
+  </si>
+  <si>
     <t>booked</t>
   </si>
   <si>
-    <t>adfa</t>
-  </si>
-  <si>
-    <t>asdfadsf</t>
-  </si>
-  <si>
-    <t>123213</t>
-  </si>
-  <si>
-    <t>adsfadsf</t>
-  </si>
-  <si>
-    <t>ej6iw</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>King</t>
-  </si>
-  <si>
-    <t>224</t>
-  </si>
-  <si>
-    <t>2023-11-28</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>asdffd</t>
-  </si>
-  <si>
-    <t>0H1Tb</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>Double</t>
-  </si>
-  <si>
-    <t>$160</t>
-  </si>
-  <si>
-    <t>adsf</t>
-  </si>
-  <si>
-    <t>12/32</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>05J79</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>asdfsdaf</t>
-  </si>
-  <si>
-    <t>dsfa1</t>
-  </si>
-  <si>
-    <t>231</t>
-  </si>
-  <si>
-    <t>sadfsda</t>
-  </si>
-  <si>
-    <t>sdafas</t>
-  </si>
-  <si>
-    <t>12321</t>
-  </si>
-  <si>
-    <t>23/43</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>uBydR</t>
-  </si>
-  <si>
-    <t>2023-11-30</t>
+    <t>jose</t>
+  </si>
+  <si>
+    <t>godinez</t>
+  </si>
+  <si>
+    <t>jogodinez25@gmail.com</t>
+  </si>
+  <si>
+    <t>1231854854</t>
+  </si>
+  <si>
+    <t>15151621</t>
+  </si>
+  <si>
+    <t>12/12</t>
+  </si>
+  <si>
+    <t>fsgfd</t>
+  </si>
+  <si>
+    <t>90065</t>
+  </si>
+  <si>
+    <t>W1vtm</t>
   </si>
 </sst>
 </file>
@@ -1230,16 +1256,16 @@
   <sheetPr/>
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="10.5714285714286"/>
-    <col min="8" max="8" width="9.57142857142857"/>
+    <col min="6" max="6" width="10.5740740740741"/>
+    <col min="8" max="8" width="9.57407407407407"/>
     <col min="11" max="11" style="6" width="9.0"/>
-    <col min="15" max="15" customWidth="true" width="13.447619047619"/>
+    <col min="15" max="15" customWidth="true" width="13.4444444444444"/>
     <col min="16" max="16" customWidth="true" width="14.3333333333333"/>
   </cols>
   <sheetData>
@@ -1464,21 +1490,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:18">
       <c r="A5" s="0">
         <v>4</v>
       </c>
       <c r="B5" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>50</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>51</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>32</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s" s="0">
         <v>19</v>
@@ -1487,40 +1513,40 @@
         <v>32</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I5" t="s" s="0">
         <v>45</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="K5" t="s" s="6">
+        <v>52</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>18</v>
       </c>
       <c r="L5" t="s" s="0">
         <v>18</v>
       </c>
       <c r="M5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="N5" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="N5" t="s" s="0">
+      <c r="O5" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="O5" t="s" s="0">
+      <c r="P5" t="s" s="0">
         <v>56</v>
-      </c>
-      <c r="P5" t="s" s="0">
-        <v>57</v>
       </c>
       <c r="Q5" t="s" s="0">
         <v>29</v>
       </c>
       <c r="R5" t="s" s="0">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="0">
         <v>5</v>
       </c>
@@ -1534,7 +1560,7 @@
         <v>17</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s" s="0">
         <v>17</v>
@@ -1543,43 +1569,42 @@
         <v>17</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I6" t="s" s="0">
         <v>36</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="K6" t="s" s="6">
+        <v>60</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>18</v>
       </c>
       <c r="L6" t="s" s="0">
         <v>18</v>
       </c>
       <c r="M6" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="N6" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="N6" t="s" s="0">
+      <c r="O6" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="O6" t="s" s="0">
+      <c r="P6" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="P6" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="Q6" s="0"/>
       <c r="R6" t="s" s="0">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:18">
       <c r="A7" s="0">
         <v>6</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>17</v>
@@ -1600,28 +1625,28 @@
         <v>18</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J7" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K7" t="s" s="6">
+      <c r="K7" s="6" t="s">
         <v>18</v>
       </c>
       <c r="L7" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="M7" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="M7" t="s" s="0">
+      <c r="N7" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="N7" t="s" s="0">
-        <v>70</v>
-      </c>
       <c r="O7" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="P7" t="s" s="0">
         <v>56</v>
-      </c>
-      <c r="P7" t="s" s="0">
-        <v>57</v>
       </c>
       <c r="Q7" t="s" s="0">
         <v>40</v>
@@ -1630,66 +1655,83 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:18">
       <c r="A8" s="0">
         <v>7</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>32</v>
       </c>
       <c r="D8" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E8" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="F8" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="F8" t="s" s="0">
+      <c r="G8" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="G8" t="s" s="0">
+      <c r="H8" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="H8" t="s" s="0">
+      <c r="I8" t="s" s="0">
         <v>76</v>
-      </c>
-      <c r="I8" t="s" s="0">
-        <v>77</v>
       </c>
       <c r="J8" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="K8" t="s" s="6">
+      <c r="K8" s="6" t="s">
         <v>18</v>
       </c>
       <c r="L8" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="M8" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="M8" t="s" s="0">
+      <c r="N8" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="P8" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="Q8" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="R8" t="s" s="0">
         <v>79</v>
-      </c>
-      <c r="N8" t="s" s="0">
-        <v>63</v>
-      </c>
-      <c r="O8" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="P8" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="Q8" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="R8" t="s" s="0">
-        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="0">
         <v>8</v>
       </c>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="N9" s="0"/>
+      <c r="O9" s="0"/>
+      <c r="P9" s="0"/>
+      <c r="Q9" s="0"/>
+      <c r="R9" s="0"/>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="0">
@@ -1912,14 +1954,14 @@
   <sheetPr/>
   <dimension ref="A1:T136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" style="1" width="11.4285714285714"/>
-    <col min="2" max="2" width="11.4285714285714"/>
+    <col min="1" max="1" style="1" width="11.4259259259259"/>
+    <col min="2" max="2" width="11.4259259259259"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20">
@@ -2010,76 +2052,64 @@
       <c r="A7" s="1">
         <v>45250</v>
       </c>
-      <c r="O7" t="s" s="0">
-        <v>49</v>
+      <c r="H7" t="s" s="0">
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1">
         <v>45251</v>
       </c>
-      <c r="N8" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="O8" t="s" s="0">
-        <v>49</v>
+      <c r="H8" t="s" s="0">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1">
         <v>45252</v>
       </c>
-      <c r="N9" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="O9" t="s" s="0">
-        <v>49</v>
+      <c r="H9" t="s" s="0">
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1">
         <v>45253</v>
       </c>
-      <c r="N10" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="O10" t="s" s="0">
-        <v>49</v>
+      <c r="H10" t="s" s="0">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1">
         <v>45254</v>
       </c>
-      <c r="N11" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="O11" t="s" s="0">
-        <v>49</v>
+      <c r="H11" t="s" s="0">
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1">
         <v>45255</v>
       </c>
-      <c r="N12" t="s" s="0">
-        <v>49</v>
+      <c r="H12" t="s" s="0">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1">
         <v>45256</v>
       </c>
-      <c r="N13" t="s" s="0">
-        <v>49</v>
+      <c r="H13" t="s" s="0">
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1">
         <v>45257</v>
       </c>
-      <c r="N14" t="s" s="0">
-        <v>49</v>
+      <c r="H14" t="s" s="0">
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:1">
@@ -2087,10 +2117,7 @@
         <v>45258</v>
       </c>
       <c r="H15" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="N15" t="s" s="0">
-        <v>49</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:1">
@@ -2098,7 +2125,7 @@
         <v>45259</v>
       </c>
       <c r="H16" t="s" s="0">
-        <v>49</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -2106,7 +2133,7 @@
         <v>45260</v>
       </c>
       <c r="H17" t="s" s="0">
-        <v>49</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:1">

</xml_diff>

<commit_message>
updated code and fixed erros
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="121">
   <si>
     <t>First Name</t>
   </si>
@@ -56,10 +56,10 @@
     <t>Room #</t>
   </si>
   <si>
-    <t>Room Size</t>
-  </si>
-  <si>
-    <t>Price</t>
+    <t>Room Type</t>
+  </si>
+  <si>
+    <t>Room Price</t>
   </si>
   <si>
     <t>Start Date</t>
@@ -68,55 +68,316 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>lil</t>
-  </si>
-  <si>
-    <t>dsfjbjksd</t>
-  </si>
-  <si>
-    <t>nwahba02@gmail.com</t>
+    <t>asjfh</t>
+  </si>
+  <si>
+    <t>sjdkfh</t>
+  </si>
+  <si>
+    <t>shfd</t>
+  </si>
+  <si>
+    <t>12344</t>
+  </si>
+  <si>
+    <t>asdfs</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>12/23</t>
+  </si>
+  <si>
+    <t>sdfhj</t>
+  </si>
+  <si>
+    <t>REMOVED</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
+  </si>
+  <si>
+    <t>changed</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>dsjfh</t>
+  </si>
+  <si>
+    <t>szjdf</t>
+  </si>
+  <si>
+    <t>sdjfk</t>
   </si>
   <si>
     <t>123</t>
   </si>
   <si>
-    <t>asdfjkasbf</t>
-  </si>
-  <si>
-    <t>djsbfhjsd</t>
-  </si>
-  <si>
-    <t>231421</t>
-  </si>
-  <si>
-    <t>12/23/12/23</t>
-  </si>
-  <si>
-    <t>sdfnsa</t>
-  </si>
-  <si>
-    <t>2424</t>
-  </si>
-  <si>
-    <t>1244</t>
-  </si>
-  <si>
-    <t>LHEnE</t>
+    <t>kuC6X</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>$115</t>
+  </si>
+  <si>
+    <t>2023-11-22</t>
+  </si>
+  <si>
+    <t>2023-11-24</t>
+  </si>
+  <si>
+    <t>making</t>
+  </si>
+  <si>
+    <t>changes</t>
+  </si>
+  <si>
+    <t>dsjfkh</t>
+  </si>
+  <si>
+    <t>asdfj</t>
+  </si>
+  <si>
+    <t>sdjf</t>
+  </si>
+  <si>
+    <t>sdfjk</t>
+  </si>
+  <si>
+    <t>1233</t>
+  </si>
+  <si>
+    <t>Dh2mJ</t>
+  </si>
+  <si>
+    <t>asdfkjb</t>
+  </si>
+  <si>
+    <t>sdjfh</t>
+  </si>
+  <si>
+    <t>sdfjkh</t>
+  </si>
+  <si>
+    <t>asdfjk</t>
+  </si>
+  <si>
+    <t>sdjkfh</t>
+  </si>
+  <si>
+    <t>sdjkf</t>
+  </si>
+  <si>
+    <t>0ks1w</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>$160</t>
+  </si>
+  <si>
+    <t>2023-12-05</t>
+  </si>
+  <si>
+    <t>2023-11-29</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>12/2</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>Suite</t>
+  </si>
+  <si>
+    <t>$1000</t>
+  </si>
+  <si>
+    <t>zsfsdj</t>
+  </si>
+  <si>
+    <t>sdj</t>
+  </si>
+  <si>
+    <t>sdjh</t>
+  </si>
+  <si>
+    <t>dsjh</t>
+  </si>
+  <si>
+    <t>dj</t>
+  </si>
+  <si>
+    <t>neXA8</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>jsdkh</t>
+  </si>
+  <si>
+    <t>ads</t>
+  </si>
+  <si>
+    <t>dsaf</t>
+  </si>
+  <si>
+    <t>kft3T</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>2023-11-28</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>sjeh</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>tRiHc</t>
+  </si>
+  <si>
+    <t>zd</t>
+  </si>
+  <si>
+    <t>V3YJG</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>CHANGE</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>2023-11-28</t>
-  </si>
-  <si>
-    <t>2023-12-01</t>
+    <t>f</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>1/2</t>
+  </si>
+  <si>
+    <t>ietpX</t>
+  </si>
+  <si>
+    <t>sj</t>
+  </si>
+  <si>
+    <t>dsj</t>
+  </si>
+  <si>
+    <t>dfj</t>
+  </si>
+  <si>
+    <t>djCX</t>
+  </si>
+  <si>
+    <t>dk</t>
+  </si>
+  <si>
+    <t>12/12</t>
+  </si>
+  <si>
+    <t>sdkj</t>
+  </si>
+  <si>
+    <t>2gtFV</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>dsf</t>
+  </si>
+  <si>
+    <t>dfs</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>frQr8</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>sdfjh</t>
+  </si>
+  <si>
+    <t>adsf</t>
+  </si>
+  <si>
+    <t>123/12</t>
+  </si>
+  <si>
+    <t>BBBBB</t>
   </si>
   <si>
     <t>booked</t>
+  </si>
+  <si>
+    <t>dsfj</t>
+  </si>
+  <si>
+    <t>12/34</t>
+  </si>
+  <si>
+    <t>1f3Sa</t>
   </si>
 </sst>
 </file>
@@ -124,11 +385,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -167,11 +428,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -182,16 +443,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -208,21 +469,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -235,17 +489,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,22 +512,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -296,16 +542,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -320,7 +581,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,7 +629,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,43 +647,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,13 +677,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,19 +707,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,67 +761,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,17 +784,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,21 +804,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -594,11 +834,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -614,148 +875,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1089,369 +1350,1134 @@
   <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="6" max="6" width="10.5703125"/>
     <col min="8" max="8" width="9.5703125"/>
-    <col min="11" max="11" width="9" style="6"/>
-    <col min="15" max="15" width="13.4453125" customWidth="1"/>
-    <col min="16" max="16" width="14.3359375" customWidth="1"/>
+    <col min="11" max="11" style="6" width="9.0"/>
+    <col min="15" max="15" customWidth="true" width="13.4453125"/>
+    <col min="16" max="16" customWidth="true" width="14.3359375"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18">
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>8</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" t="s" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>25</v>
       </c>
       <c r="K2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q3" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="R3" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="R2" t="s">
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="N4" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="P4" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="Q4" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="R4" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6">
+      <c r="C5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="M5" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="N5" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="O5" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="P5" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="Q5" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="R5" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7">
+      <c r="B6" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="O6" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="Q6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="R6" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8">
+      <c r="B7" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="M7" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="N7" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="O7" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="P7" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="Q7" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="R7" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9">
+      <c r="B8" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="M8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="N8" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="P8" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="Q8" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="R8" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="0">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10">
+      <c r="B9" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="M9" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="N9" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="O9" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="P9" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="Q9" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="R9" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11">
+      <c r="B10" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="M10" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="N10" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="O10" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="P10" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="Q10" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="R10" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="0">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12">
+      <c r="B11" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="M11" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="N11" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="O11" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="P11" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="Q11" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="R11" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="0">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13">
+      <c r="B12" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="M12" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="N12" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="O12" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="P12" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="Q12" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="R12" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="0">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14">
+      <c r="B13" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="L13" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="M13" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="N13" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="O13" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="P13" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="Q13" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="R13" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="0">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15">
+      <c r="B14" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="G14" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="H14" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="I14" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="J14" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="M14" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="N14" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="O14" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="P14" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="Q14" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="R14" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="0">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16">
+      <c r="B15" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="H15" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="I15" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="J15" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="M15" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="N15" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="O15" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="P15" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="Q15" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="R15" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="0">
         <v>15</v>
       </c>
+      <c r="B16" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="G16" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="H16" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="I16" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="J16" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="M16" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="N16" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="O16" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="P16" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="Q16" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="R16" t="s" s="0">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>16</v>
       </c>
+      <c r="B17" t="s" s="0">
+        <v>118</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="H17" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="I17" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="J17" t="s" s="0">
+        <v>118</v>
+      </c>
+      <c r="K17" t="s" s="6">
+        <v>37</v>
+      </c>
+      <c r="L17" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="M17" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="N17" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="O17" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="P17" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="Q17" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="R17" t="s" s="0">
+        <v>63</v>
+      </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27">
+      <c r="A27" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28">
+      <c r="A28" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29">
+      <c r="A29" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30">
+      <c r="A30" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31">
+      <c r="A31" s="0">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32">
+      <c r="A32" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33">
+      <c r="A33" s="0">
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34">
+      <c r="A34" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35">
+      <c r="A35" s="0">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36">
+      <c r="A36" s="0">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37">
+      <c r="A37" s="0">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38">
+      <c r="A38" s="0">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39">
+      <c r="A39" s="0">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40">
+      <c r="A40" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41">
+      <c r="A41" s="0">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42">
+      <c r="A42" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43">
+      <c r="A43" s="0">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44">
+      <c r="A44" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45">
+      <c r="A45" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46">
+      <c r="A46" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47">
+      <c r="A47" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48">
+      <c r="A48" s="0">
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49">
+      <c r="A49" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50">
+      <c r="A50" s="0">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51">
+      <c r="A51" s="0">
         <v>50</v>
       </c>
     </row>
@@ -1467,12 +2493,12 @@
   <dimension ref="A1:T136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="11.4296875" style="1"/>
+    <col min="1" max="1" style="1" width="11.4296875"/>
     <col min="2" max="2" width="11.4296875"/>
   </cols>
   <sheetData>
@@ -1560,144 +2586,67 @@
         <v>45249</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:1">
       <c r="A7" s="1">
         <v>45250</v>
       </c>
-      <c r="H7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+    </row>
+    <row r="8" spans="1:1">
       <c r="A8" s="1">
         <v>45251</v>
       </c>
-      <c r="H8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+    </row>
+    <row r="9" spans="1:1">
       <c r="A9" s="1">
         <v>45252</v>
       </c>
-      <c r="H9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+    </row>
+    <row r="10" spans="1:1">
       <c r="A10" s="1">
         <v>45253</v>
       </c>
-      <c r="H10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+    </row>
+    <row r="11" spans="1:1">
       <c r="A11" s="1">
         <v>45254</v>
       </c>
-      <c r="H11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+    </row>
+    <row r="12" spans="1:1">
       <c r="A12" s="1">
         <v>45255</v>
       </c>
-      <c r="H12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+    </row>
+    <row r="13" spans="1:1">
       <c r="A13" s="1">
         <v>45256</v>
-      </c>
-      <c r="H13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>45257</v>
       </c>
-      <c r="E14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" t="s">
-        <v>33</v>
-      </c>
+      <c r="B14" s="0"/>
+      <c r="H14" s="0"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>45258</v>
       </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" t="s">
-        <v>33</v>
-      </c>
+      <c r="B15" s="0"/>
+      <c r="H15" s="0"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>45259</v>
       </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" t="s">
-        <v>33</v>
-      </c>
+      <c r="B16" s="0"/>
+      <c r="H16" s="0"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>45260</v>
       </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" t="s">
-        <v>33</v>
-      </c>
+      <c r="H17" s="0"/>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1">

</xml_diff>

<commit_message>
cleaned up the gui and fixed the grouped radio buttons will start work on admin login now
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="122">
   <si>
     <t>First Name</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>1f3Sa</t>
+  </si>
+  <si>
+    <t>2023-12-01</t>
   </si>
 </sst>
 </file>
@@ -2062,7 +2065,7 @@
       <c r="J13" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="K13" t="s" s="6">
         <v>94</v>
       </c>
       <c r="L13" t="s" s="0">
@@ -2072,19 +2075,19 @@
         <v>98</v>
       </c>
       <c r="N13" t="s" s="0">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="O13" t="s" s="0">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="P13" t="s" s="0">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="Q13" t="s" s="0">
         <v>30</v>
       </c>
       <c r="R13" t="s" s="0">
-        <v>31</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -2626,31 +2629,42 @@
         <v>45257</v>
       </c>
       <c r="B14" s="0"/>
-      <c r="H14" s="0"/>
+      <c r="H14" t="s" s="0">
+        <v>117</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>45258</v>
       </c>
       <c r="B15" s="0"/>
-      <c r="H15" s="0"/>
+      <c r="H15" t="s" s="0">
+        <v>117</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>45259</v>
       </c>
       <c r="B16" s="0"/>
-      <c r="H16" s="0"/>
+      <c r="H16" t="s" s="0">
+        <v>117</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>45260</v>
       </c>
-      <c r="H17" s="0"/>
+      <c r="H17" t="s" s="0">
+        <v>117</v>
+      </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1">
         <v>45261</v>
+      </c>
+      <c r="H18" t="s" s="0">
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:1">

</xml_diff>

<commit_message>
Fixes to some error's and some comments
</commit_message>
<xml_diff>
--- a/HotelProject/Hotel Project.xlsx
+++ b/HotelProject/Hotel Project.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="131">
   <si>
     <t>First Name</t>
   </si>
@@ -381,6 +381,33 @@
   </si>
   <si>
     <t>2023-12-01</t>
+  </si>
+  <si>
+    <t>joef</t>
+  </si>
+  <si>
+    <t>fjisdk</t>
+  </si>
+  <si>
+    <t>jogodinez25@yahoo.com</t>
+  </si>
+  <si>
+    <t>jo</t>
+  </si>
+  <si>
+    <t>1234123412341234</t>
+  </si>
+  <si>
+    <t>fdsfd</t>
+  </si>
+  <si>
+    <t>90065</t>
+  </si>
+  <si>
+    <t>Aqd3j</t>
+  </si>
+  <si>
+    <t>2023-11-25</t>
   </si>
 </sst>
 </file>
@@ -2318,6 +2345,57 @@
       <c r="A18" s="0">
         <v>17</v>
       </c>
+      <c r="B18" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>123</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>124</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="G18" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="H18" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="I18" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="J18" t="s" s="0">
+        <v>127</v>
+      </c>
+      <c r="K18" t="s" s="6">
+        <v>128</v>
+      </c>
+      <c r="L18" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="M18" t="s" s="0">
+        <v>129</v>
+      </c>
+      <c r="N18" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="O18" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="P18" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="Q18" t="s" s="0">
+        <v>130</v>
+      </c>
+      <c r="R18" t="s" s="0">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="0">
@@ -2618,11 +2696,17 @@
       <c r="A12" s="1">
         <v>45255</v>
       </c>
+      <c r="N12" t="s" s="0">
+        <v>117</v>
+      </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1">
         <v>45256</v>
       </c>
+      <c r="N13" t="s" s="0">
+        <v>117</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1">
@@ -2632,6 +2716,9 @@
       <c r="H14" t="s" s="0">
         <v>117</v>
       </c>
+      <c r="N14" t="s" s="0">
+        <v>117</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1">
@@ -2641,6 +2728,9 @@
       <c r="H15" t="s" s="0">
         <v>117</v>
       </c>
+      <c r="N15" t="s" s="0">
+        <v>117</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1">
@@ -2650,12 +2740,18 @@
       <c r="H16" t="s" s="0">
         <v>117</v>
       </c>
+      <c r="N16" t="s" s="0">
+        <v>117</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>45260</v>
       </c>
       <c r="H17" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="N17" t="s" s="0">
         <v>117</v>
       </c>
     </row>

</xml_diff>